<commit_message>
adding specific chrome user argument
</commit_message>
<xml_diff>
--- a/Website/static/amazon/Amazon Web-Scraper.xlsx
+++ b/Website/static/amazon/Amazon Web-Scraper.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -25,196 +25,373 @@
     <t>Search Term</t>
   </si>
   <si>
+    <t>Wireless Earbuds, UMIDIGI AirBuds U Wireless Headphones with Microphones, Bluetooth 5.1 Earphones in-Ear, Touch Control Bluetooth Earbuds, 24H Playing Time for Work and Home Office.</t>
+  </si>
+  <si>
+    <t>Truly Wireless Earbuds, Tronsmart Noise Cancelling Earbuds with Charging Case, Built-in Clear Call Mics, Hi-Fi Stereo Audio Bluetooth Headphones, Sensitive Touch &amp; Waterproof Earphones for Sports Gaming Work Travel</t>
+  </si>
+  <si>
+    <t>Skullcandy Dime True Wireless Earbuds, True Black (S2DMW-P740)</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, GOSCIEN Headphones Wireless Immersive Bass Sound Bluetooth 5.0 Headphones with Noise Cancellation Mic, IPX5 Waterproof Bluetooth Earphone with Charging Case for Work, Sports</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Tribit 100H Playtime Bluetooth 5.0 IPX8 Waterproof Touch Control Ture Wireless Bluetooth Earbuds with Mic Earphone in-Ear Deep Bass Built-in Mic Bluetooth Headphones, Flybuds 3</t>
+  </si>
+  <si>
+    <t>Hi-Res Extra Bass Earbuds Noise Isolating in-Ear Headphones Wired Earbuds with Microphone for iPhone, iPod, iPad, MP3, Huawei, Samsung, Lightweight Earphones with Volume Control 3.5mm Jack Headphones</t>
+  </si>
+  <si>
+    <t>Wireless Bluetooth 5.0 Earbuds Headset in-Ear Noise Canceling Sport Headphones with LED Digital Shows Charging Case,Stereo Touch Control Waterproof Earphones Built-in Mic for Workout/Running/Gym (Black)</t>
+  </si>
+  <si>
+    <t>Apple EarPods with Lightning Connector</t>
+  </si>
+  <si>
+    <t>Sony MDRZX110 Over-Ear Headphones (Black)</t>
+  </si>
+  <si>
+    <t>Sony MDREX15LP/B In-Ear Headphones (Black)</t>
+  </si>
+  <si>
+    <t>Panasonic RPTCM125V ErgoFit In-Ear Earbud Headphones with Mic and Controller, Violet</t>
+  </si>
+  <si>
+    <t>Sennheiser CX 300S in Ear Headphone with One-Button Smart Remote - Black</t>
+  </si>
+  <si>
+    <t>Monster Wireless Earbuds,Super Fast Charge,Bluetooth 5.0 in-Ear Stereo Headphones with USB-C Charging Case,Built-in Mic for Clear Calls,Water Resistant Design for Sports,Black.</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds Bluetooth 5.0 Headphones,40H Playtime w/Wireless Charging Case,IP6 Waterproof/Button Control/TWS Stereo Bluetooth Earphones in-Ear w/Mic for Running Workout Gym</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, AIKELA Bluetooth 5.1 Earbuds Waterproof Touch Control Wireless Earphones with Hi-Fi Stereo Audio, Type-C Quick Charging Case, 15H Playtime, Single/Twin Mode, Built-in Mic for Gym, Home, Office</t>
+  </si>
+  <si>
+    <t>Wireless Bluetooth earbuds, Bluetooth 5.0 in-ear headphones, 6D stereo IPX5 sweatproof, clear binaural call microphone, fitness, entertainment time charging box, noise reduction mini earbuds, sweatproof for mobile phones and Android Gym Sport（Black）</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Bluetooth Earbuds Bass+ Stereo Sound/USB-C Fast Charging/28H Playtime/IPX7 Waterproof Wireless Earphones Sport Headphones in Ear Bluetooth Earphones with Mic for Workout Gym (Black)</t>
+  </si>
+  <si>
     <t>OKIMO Wireless Earbuds Bluetooth 5 Headphones with 3500mAh LED Charging Case, IPX7 Waterproof TWS Stereo Earphones in Ear, Hands-Free Headset with Mic, Touch Control, 125 Hours Playback for for Work / Home Office (Black)</t>
   </si>
   <si>
-    <t>Truly Wireless Earbuds, Tronsmart Noise Cancelling Earbuds with Charging Case, Built-in Clear Call Mics, Hi-Fi Stereo Audio Bluetooth Headphones, Sensitive Touch &amp; Waterproof Earphones for Sports Gaming Work Travel</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, GOSCIEN Headphones Wireless Immersive Bass Sound Bluetooth 5.0 Headphones with Noise Cancellation Mic, IPX5 Waterproof Bluetooth Earphone with Charging Case for Work, Sports</t>
-  </si>
-  <si>
-    <t>Sport Headphones with Earhook Design, APEKX True Wireless Bluetooth 5.0 Sports Earbuds, IPX7 Waterproof Stereo Sound, Built-in Mic Earphones with Portable Charging Case Supporting Wireless Charging(Black)</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Tribit 100H Playtime Bluetooth 5.0 IPX8 Waterproof Touch Control Ture Wireless Bluetooth Earbuds with Mic Earphone in-Ear Deep Bass Built-in Mic Bluetooth Headphones, Flybuds 3</t>
-  </si>
-  <si>
     <t>Monster Wireless Earbuds, Bluetooth 5.0 in-Ear Stereo Headphones, Built-in Mics for Clear Calls, USB-C Quick Charge, 24-Hour Playtime, Single/Twin Mode for iPhone/Android</t>
   </si>
   <si>
-    <t>Monster Wireless Earbuds,Super Fast Charge,Bluetooth 5.0 in-Ear Stereo Headphones with USB-C Charging Case,Built-in Mic for Clear Calls,Water Resistant Design for Sports,Black.</t>
+    <t>Anker Soundcore Life P2 True Wireless Earbuds with 4 Microphones,CVC 8.0 Noise Reduction, Graphene Driver, Clear Sound, USB C, 40H Playtime, IPX7 Waterproof, Wireless Earphones for Work, Home Office</t>
+  </si>
+  <si>
+    <t>Vipcall Wireless Earbuds, in-Ear Bluetooth Headphones, Immersive Bass Sound, IPX8 Waterproof Sport Earphones, Touch Control Bluetooth Earbuds, 25 Hrs w/USB-C Charging Case/Twin&amp;Mono Mode/Mics, Black</t>
+  </si>
+  <si>
+    <t>Apple EarPods with 3.5mm Headphone Plug</t>
+  </si>
+  <si>
+    <t>Apple AirPods with Charging Case</t>
+  </si>
+  <si>
+    <t>Monster Mission V1 Wireless Earbuds, Bluetooth 5.0 Built-in Mic Noise Cancelling Gaming Earbuds, Cool Light Effects with Music &amp; Game Modes, 48ms Ultra Low-Latency Gaming Earphones (Black)</t>
+  </si>
+  <si>
+    <t>Otium Wireless Earbuds Bluetooth 5.0 Headphones with Digital Intelligence LED Display 3500 mAH Charging Case 135H Playtime Stereo Sound Headset IPX8 Waterproof Built-in Mic for Home Office</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Bluetooth 5.1 Wireless Headphones in-Ear Stereo Sports Bluetooth Earphones, Noise Cancelling Earbuds with Mic Deep Bass, IPX7 Waterproof, 40H Playtime Wireless Headset for Sports</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, 48Hours Playtime True Wireless Bluetooth Earbuds Noise Reduction Stereo Call Built-in Mics Wireless Earphones Extra Bass Sound E90 Wireless Headphones Waterpoof IPX8 Bluetooth V5.0 Headsets with Type-C Port Charging Case</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, MDots Bluetooth Earbuds Immersive Stereo Sound, Bluetooth Earphones Twin&amp;Mono Mode, Wireless Headphones in Ear with Microphones/Precise Button Control/IPX6 Waterproof for Sport</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds,AXLOIE Active Noise Cancelling Bluetooth Earphones,in-Ear Wireless Headphones with 4-Mic Clear Call,ANC Stereo Earbuds Premium Deep Bass,with Portable Charging Case,19H Playtime</t>
+  </si>
+  <si>
+    <t>Apple AirPods Pro</t>
+  </si>
+  <si>
+    <t>GO5 Mini Wireless Earbuds Bluetooth Headphones Premium Fidelity Sound Quality Wireless Charging Case Digital LED Intelligence Display IPX7 Waterproof Earphones Built-in Mic Headset for Sport Black</t>
+  </si>
+  <si>
+    <t>JBL Tune 125TWS True Wireless In-Ear Bluetooth Headphones with up to 32 Hours of Combined Music Playtime - Black</t>
+  </si>
+  <si>
+    <t>Sony MDR-XB50AP/B Extra Bass Earbud Headphones (Black)</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Bluetooth Earbuds with CVC8.0 Noise Cancelling Mics, 35H Playtime/Deep Bass/USB-C Quick Charge/Touch Control, IPX8 Waterproof Headphones for Work Sport</t>
+  </si>
+  <si>
+    <t>True Wireless Earbuds, Bluetooth 5.0 in-Ear Headphones with Charging Box, IPX7 Waterproof Stereo Headphones in-Ear Earphones, Headset Built in Mic, Premium Sound with Deep Bass, Sport/Work</t>
   </si>
   <si>
     <t>JUKSTG Earphones Noise Isolating in-Ear Headphones with Pure Sound and Powerful Bass with High Sensitivity Microphone and Volume Control</t>
   </si>
   <si>
-    <t>Hi-Res Extra Bass Earbuds Noise Isolating in-Ear Headphones Wired Earbuds with Microphone for iPhone, iPod, iPad, MP3, Huawei, Samsung, Lightweight Earphones with Volume Control 3.5mm Jack Headphones</t>
+    <t>ULIX Rider Earphones in-Ear Headphones with Mic, 3 Years Warranty, with Anti-Tangle, Braided Cable, Microphone, Super Resistant, 48 Ω Driver, Intense Bass, Earbuds for Samsung, Computer, Laptop</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Buds Live (Black) - True Wireless, Active Noise Cancelling, Wireless Charging Case (CAD Version)</t>
+  </si>
+  <si>
+    <t>Panasonic RPHJE120K In-Ear Headphone, Black</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds Bluetooth 5.0 Wireless Headphones in-Ear Stereo Noise Cancelling Bluetooth Earbuds with LED Charging Case IPX7 Waterproof Touch Control Headset Built-in Mic Earphones for Sport/Work (black)</t>
+  </si>
+  <si>
+    <t>Wireless Bluetooth Earbuds, AIKELA Active Noise Cancelling Ear Buds with 4 Mics, Activate Voice Assistant, Hi-FI Stereo Sound in-Ear Headphones with Wireless Charging Box, Touch Control Bluetooth 5.0 Sport Earphones Support 3 Play Modes</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, MDots Bluetooth Earbuds Rhythm Stereo Sound Wireless Earphones in Ear w/20 Hrs Playtime, IPX6 Waterproof Sports Headphones with Mic Single/Twin Mode for Running, Workout</t>
+  </si>
+  <si>
+    <t>Monster Wireless Earbuds, Bluetooth 5.0 in-Ear Headphones with Charging Case, Stereo Earphones Deep Bass Sound, IPX5 Waterproof, Built-in Mic, Clear Call, Secure Fit for Sports</t>
+  </si>
+  <si>
+    <t>New Beats Studio Buds – True Wireless Noise Cancelling Earbuds – Compatible with Apple &amp; Android, Built-in Microphone, IPX4 Rating, Sweat Resistant Earphones, Class 1 Bluetooth Headphones - Black</t>
+  </si>
+  <si>
+    <t>ULIX Rider Earphones in-Ear Headphones with Mic, 3 Years Warranty, with Anti-Tangle, Reinforced Cable, Microphone, Super Resistant, 48 Ω Driver, Intense Bass, Earbuds for Samsung, Computer, Laptop</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Buds Pro - Black</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds Active Noise Cancellation, Bluetooth Earbuds 32 Hours Cycle Playtime with Type-C Charging Case Smart Touch ANC Wireless Earphones, Built-in 4Mics Bluetooth V5.0 Headsets Stereo Call, Deep Bass Sound A9 Wireless Headphones with IPX7 Waterproof for Outdoor Sport</t>
+  </si>
+  <si>
+    <t>Bluetooth Earbuds, Wireless Earbuds Pink, Deep Bass Bluetooth Earphones w/Ergonomic Design/Mono&amp;Twin Mode/25 Hrs/IPX8 Waterproof/Microphones/Type-C Charging for Sport</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds SoundPEATS T2 Bluetooth Earphone Hybrid Active Noise Cancelling, ANC Earphones with Transparency Mode, Bluetooth 5.1 in-Ear Headphones, 30 Hours Playtime, USB-C Quick Charge, Stereo Sound, 12mm Driver</t>
+  </si>
+  <si>
+    <t>MMK Wireless Earbuds with Mic and Wireless Charge, 5.1 Bluetooth Touch Contral, IPX8 Waterproof In-Ear Earphone with CVC 8.0 Noise Cancelling, Built-in TWS Stereo Headphones with Deep Bass for Sport/ Work</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds SoundPEATS TrueAir2 Earphones Bluetooth V5.2 with 4 Mic, CVC Noise Cancellation for Clear Calls Headphones Qualcomm 3040, aptX Codec, USB C, 25 Hours Playtime</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Bluetooth 5.0 Earbuds Waterproof Wireless Earphones, with 35H Playtime, Hi-Fi Audio Deep Bass, Noise-Canceling Mic, in-Ear Ear Buds with Charging Case, Sensitive Touch Control Bluetooth Sport Earphones, for Samsung/iPhone/Android</t>
+  </si>
+  <si>
+    <t>iKanzi Wireless Earbuds Bluetooth 5 Headphones with Charging Case, IPX7 Waterproof TWS Stereo Earphones in Ear, Hands-Free Headset with Mic, Touch Control, USB-C Fast Charging, 25 Hours Playback for iPhone and Android (black)</t>
+  </si>
+  <si>
+    <t>True Wireless Earbuds, in-Ear Bluetooth Earbuds , with Fast Charging Case Noise Canceling 3D Stereo Headsets Touch Control Headphones, HD Stereo Deep Bass Built-in Mic Waterproof Gym Sports Earphones (Black)</t>
+  </si>
+  <si>
+    <t>2021 Wireless Earbuds, Tribit Qualcomm QCC3040 Bluetooth 5.2, 4 Mics CVC 8.0 Call Noise Reduction 50H Playtime Clear Calls Volume Control True Wireless Bluetooth Earbuds Earphones, FlyBuds C1</t>
   </si>
   <si>
     <t>2 Pack Earbuds/Headphones/Earphones with 3.5mm Wired in Ear Headphone Plug(Built-in Microphone &amp; Volume Control) Compatible with iPhone,iPad,iPod,PC,MP3/4,Android -White</t>
   </si>
   <si>
-    <t>Apple EarPods with Lightning Connector</t>
-  </si>
-  <si>
-    <t>Sony MDREX15LP/B In-Ear Headphones (Black)</t>
-  </si>
-  <si>
-    <t>Panasonic RPHJE120K In-Ear Headphone, Black</t>
-  </si>
-  <si>
-    <t>AmazonBasics In-Ear Wired Headphones, Earbuds with Microphone, Black</t>
-  </si>
-  <si>
-    <t>slitinto Wireless Earbuds Bluetooth 5.0 Earphones, IPX7 Waterproof Bluetooth Earbuds with 30H Playtime, TWS Stereo in-Ear Sports Headset with Charging Case, Mic, Touch Control for Running/Workout</t>
-  </si>
-  <si>
-    <t>Donerton Wireless Earbuds, Bluetooth 5.0 Headphones IP8 Waterproof Earbuds, 80 Playtime, in Ear Earphones with Mic, Deep Bass 3D Stereo, Charging Case, Sports, Work Out, Easy Pairing, Power Bank</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds Bluetooth 5.1 Earphones, pendali IPX7 Waterproof Earbuds with Deep Bass, Auto Pairing, Mini Portable Charging Case, Touch Control in-Ear Wireless Headphones for Sport Running</t>
-  </si>
-  <si>
-    <t>Wireless Bluetooth 5.0 Earbuds Headset in-Ear Noise Canceling Sport Headphones with LED Digital Shows Charging Case,Stereo Touch Control Waterproof Earphones Built-in Mic for Workout/Running/Gym (Black)</t>
-  </si>
-  <si>
-    <t>Wireless Bluetooth earbuds, Bluetooth 5.0 in-ear headphones, 6D stereo IPX5 sweatproof, clear binaural call microphone, fitness, entertainment time charging box, noise reduction mini earbuds, sweatproof for mobile phones and Android Gym Sport（Black）</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, UMIDIGI AirBuds U Wireless Headphones with Microphones, Bluetooth 5.1 Earphones in-Ear, Touch Control Bluetooth Earbuds, 24H Playing Time for Work and Home Office.</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Bluetooth Earbuds Bass+ Stereo Sound/USB-C Fast Charging/28H Playtime/IPX7 Waterproof Wireless Earphones Sport Headphones in Ear Bluetooth Earphones with Mic for Workout Gym (Black)</t>
-  </si>
-  <si>
-    <t>Skullcandy Dime True Wireless Earbuds, True Black (S2DMW-P740)</t>
-  </si>
-  <si>
-    <t>Monster Wireless Earbuds, Bluetooth 5.0 in-Ear Headphones with Charging Case, Stereo Earphones Deep Bass Sound, IPX5 Waterproof, Built-in Mic, Clear Call, Secure Fit for Sports</t>
-  </si>
-  <si>
-    <t>NYZ M9 Wireless Earbuds,True Wireless Bluetooth Earbuds Hi-Fi Stereo Bass Headphones in-Ear Earphones LED Display Charging Case with Mic CVC 8.0 in-Ear Protection for Working/Travel/Gym</t>
-  </si>
-  <si>
-    <t>JBL Tune 125TWS True Wireless In-Ear Bluetooth Headphones with up to 32 Hours of Combined Music Playtime - Black</t>
-  </si>
-  <si>
-    <t>Apple EarPods with 3.5mm Headphone Plug</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Buds Pro - Black</t>
-  </si>
-  <si>
-    <t>Apple AirPods with Charging Case</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Bluetooth 5.1 Wireless Headphones in-Ear Stereo Sports Bluetooth Earphones, Noise Cancelling Earbuds with Mic Deep Bass, IPX7 Waterproof, 40H Playtime Wireless Headset for Sports</t>
-  </si>
-  <si>
-    <t>TCL S200 True Wireless Earbuds with 4 Microphones, Bluetooth Headphones, Echo Noise Cancellation, Clear Sound, Type C Charging Case, Touch Control, Waterproof Earphones for Work, Home Office, Black</t>
+    <t>Wireless Earbuds, EarFun Air 4 Mics Noise Canceling, Bluetooth 5.0 Earbuds Touch Control, Wireless Charging, USB-C Quick Charge, Deep Bass, in-Ear Detection Headphones, 35H Playtime, IPX7 Waterproof</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, 5.0 Bluetooth Earbuds,Touch Control Cute Cat Wireless Earset with Microphone - Hi-Fi Stereo Audio, Noise Reduction, Waterproof for iPhone/Android to Kids Adult Gift</t>
+  </si>
+  <si>
+    <t>42 Hours Wireless Earbuds, Forte Wireless Earphones Bluetooth 5.0 Premium Lossless Audio with Smooth Switch Stereo or Mono, Smart Touch Bluetooth Earbuds Built-in Mics Headset, Wireless Headphones IPX8 Type-C for Sport and Travel</t>
   </si>
   <si>
     <t>Wireless Earbuds E19 Bluetooth Earbuds 15Hours Cycle Playtime with Mini Charging Case, 3D Stereo Sound Wireless Earphones Built-in Mic Headsets for Gym Sport, True Wireless Headphones for iOS and Android Bluetooth Device</t>
   </si>
   <si>
-    <t>42 Hours Wireless Earbuds, Forte Wireless Earphones Bluetooth 5.0 Premium Lossless Audio with Smooth Switch Stereo or Mono, Smart Touch Bluetooth Earbuds Built-in Mics Headset, Wireless Headphones IPX8 Type-C for Sport and Travel</t>
-  </si>
-  <si>
-    <t>Sony MDR-XB50AP/B Extra Bass Earbud Headphones (Black)</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, AIKELA Bluetooth 5.1 Earbuds Waterproof Touch Control Wireless Earphones with Hi-Fi Stereo Audio, Type-C Quick Charging Case, 15H Playtime, Single/Twin Mode, Built-in Mic for Gym, Home, Office</t>
-  </si>
-  <si>
-    <t>True Wireless Earbuds, Bluetooth 5.0 in-Ear Headphones with Charging Box, IPX7 Waterproof Stereo Headphones in-Ear Earphones, Headset Built in Mic, Premium Sound with Deep Bass, Sport/Work</t>
-  </si>
-  <si>
-    <t>Apple AirPods Pro</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds,AXLOIE Active Noise Cancelling Bluetooth Earphones,in-Ear Wireless Headphones with 4-Mic Clear Call,ANC Stereo Earbuds Premium Deep Bass,with Portable Charging Case,19H Playtime</t>
-  </si>
-  <si>
-    <t>New Beats Studio Buds – True Wireless Noise Cancelling Earbuds – Compatible with Apple &amp; Android, Built-in Microphone, IPX4 Rating, Sweat Resistant Earphones, Class 1 Bluetooth Headphones - Black</t>
-  </si>
-  <si>
-    <t>SENNHEISER Momentum True Wireless 2 - Bluetooth Earbuds with Active Noise Cancellation, Smart Pause, Customizable Touch Control and 28-Hour Battery Life - White (M3IETW2 White)</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Bluetooth Earbuds with CVC8.0 Noise Cancelling Mics, 35H Playtime/Deep Bass/USB-C Quick Charge/Touch Control, IPX8 Waterproof Headphones for Work Sport</t>
-  </si>
-  <si>
-    <t>GO5 Mini Wireless Earbuds Bluetooth Headphones Premium Fidelity Sound Quality Wireless Charging Case Digital LED Intelligence Display IPX7 Waterproof Earphones Built-in Mic Headset for Sport Black</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Buds Live (Black) - True Wireless, Active Noise Cancelling, Wireless Charging Case (CAD Version)</t>
-  </si>
-  <si>
-    <t>Anker Soundcore Life P2 True Wireless Earbuds with 4 Microphones,CVC 8.0 Noise Reduction, Graphene Driver, Clear Sound, USB C, 40H Playtime, IPX7 Waterproof, Wireless Earphones for Work, Home Office</t>
-  </si>
-  <si>
-    <t>ULIX Rider Earphones in-Ear Headphones with Mic, 3 Years Warranty, with Anti-Tangle, Braided Cable, Microphone, Super Resistant, 48 Ω Driver, Intense Bass, Earbuds for Samsung, Computer, Laptop</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Bluetooth 5.0 Earbuds Waterproof Wireless Earphones, with 35H Playtime, Hi-Fi Audio Deep Bass, Noise-Canceling Mic, in-Ear Ear Buds with Charging Case, Sensitive Touch Control Bluetooth Sport Earphones, for Samsung/iPhone/Android</t>
-  </si>
-  <si>
-    <t>Vipcall Wireless Earbuds, in-Ear Bluetooth Headphones, Immersive Bass Sound, IPX8 Waterproof Sport Earphones, Touch Control Bluetooth Earbuds, 25 Hrs w/USB-C Charging Case/Twin&amp;Mono Mode/Mics, Black</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds SoundPEATS T2 Bluetooth Earphone Hybrid Active Noise Cancelling, ANC Earphones with Transparency Mode, Bluetooth 5.1 in-Ear Headphones, 30 Hours Playtime, USB-C Quick Charge, Stereo Sound, 12mm Driver</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds Bluetooth 5.0 Wireless Headphones in-Ear Stereo Noise Cancelling Bluetooth Earbuds with LED Charging Case IPX7 Waterproof Touch Control Headset Built-in Mic Earphones for Sport/Work</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, MDots Bluetooth Earbuds Immersive Stereo Sound, Bluetooth Earphones Twin&amp;Mono Mode, Wireless Headphones in Ear with Microphones/Precise Button Control/IPX6 Waterproof for Sport</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds Bluetooth 5.0 Headphones,40H Playtime w/Wireless Charging Case,IP6 Waterproof/Button Control/TWS Stereo Bluetooth Earphones in-Ear w/Mic for Running Workout Gym</t>
-  </si>
-  <si>
-    <t>Wireless Bluetooth Earbuds, AIKELA Active Noise Cancelling Ear Buds with 4 Mics, Activate Voice Assistant, Hi-FI Stereo Sound in-Ear Headphones with Wireless Charging Box, Touch Control Bluetooth 5.0 Sport Earphones Support 3 Play Modes</t>
-  </si>
-  <si>
-    <t>APEKX Bluetooth Headphones True Wireless Earbuds with Charging Case IPX7 Waterproof TWS Stereo Sound Earphones Built-in Mic in-Ear Headsets Deep Bass for Sport Running Black</t>
-  </si>
-  <si>
-    <t>Bluetooth Earbuds, Wireless Earbuds Pink, Deep Bass Bluetooth Earphones w/Ergonomic Design/Mono&amp;Twin Mode/25 Hrs/IPX8 Waterproof/Microphones/Type-C Charging for Sport</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Bluetooth 5.0 Active Noise Cancelling Earphones 4 Built-in Mics in-Ear Earbuds with IPX5 Waterproof 19H Playtime Deep Bass for Music and Clear Calls</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, 48Hours Playtime True Wireless Bluetooth Earbuds Noise Reduction Stereo Call Built-in Mics Wireless Earphones Extra Bass Sound E90 Wireless Headphones Waterpoof IPX8 Bluetooth V5.0 Headsets with Type-C Port Charging Case</t>
-  </si>
-  <si>
-    <t>Bluetooth Headphones, Wireless Earbuds 5.0 Strong Bass Hi-Fi Stereo Headset 20H Game Time with Charging Case IPX5 Waterproof Built-in Mic,Three Size Ear Tips, Suitable for Sports Running(Black)…</t>
-  </si>
-  <si>
-    <t>SOUNDPEATS Q Wireless Earbuds Bluetooth 5.0 Wireless Earphones in-Ear Wireless Charging Headphones with 4-Mic 10mm Driver Touch Control 21Hrs Playtime USB-C Charge (Black)</t>
-  </si>
-  <si>
-    <t>ULIX Rider Earphones in-Ear Headphones with Mic, 3 Years Warranty, with Anti-Tangle, Reinforced Cable, Microphone, Super Resistant, 48 Ω Driver, Intense Bass, Earbuds for Samsung, Computer, Laptop</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds SoundPEATS TrueAir2 Earphones Bluetooth V5.2 with 4 Mic, CVC Noise Cancellation for Clear Calls Headphones Qualcomm 3040, aptX Codec, USB C, 25 Hours Playtime</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Bluetooth 5.1 Sport Headphones with Quick Release Earhook, IPX7 Waterproof in-Ear bluetooth Earphones, Type-C Charging/Auto Pairing/25H Playtime/Touch Control, Deep Bass headset for Gym</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Tronsmart Apollo Air Plus Active Noise Cancelling Earbuds with 6-Mic, in-Ear Bluetooth 5.2 Headphones, Hi-Fi Stereo Earphones, Touch Control, with Wireless/Type-C Charging Case</t>
-  </si>
-  <si>
-    <t>[Xmythorig Ultimate] True Wireless Earbuds Bluetooth 5.0 Headphones, IPX7 Waterproof Earphones for Sports, 110H Playtime w/ 3300mAh Charging Case, 3D Stereo Audio Touch Control in-Ear Headset w/Mic</t>
-  </si>
-  <si>
-    <t>Monster Mission V1 Wireless Earbuds, Bluetooth 5.0 Built-in Mic Noise Cancelling Gaming Earbuds, Cool Light Effects with Music &amp; Game Modes, 48ms Ultra Low-Latency Gaming Earphones (Black)</t>
+    <t>UMIDIGI A9 Cell Phone, 64GB Fully Unlocked Smartphone, 5150mAh Battery Android Phone with 6.53" HD+ Full Screen and 13MP AI Triple Camera (Peacock Green)</t>
+  </si>
+  <si>
+    <t>Panasonic Dect_6.0 4-Handset Landline Telephone</t>
+  </si>
+  <si>
+    <t>UMIDIGI A9 Pro Unlocked Cell Phones 6.3" FHD+ Full Screen, 4150mAh High Capacity Battery Smartphone with AI Matrix Quad Camera, Dual SIM Phone (Forest Green, 6+128GB)</t>
+  </si>
+  <si>
+    <t>Motorola ML1000 DECT 6.0 Expandable 4-line Business Phone System with Voicemail, Digital Receptionist and Music on Hold, Black</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A10e 32GB Unlocked Phone - Black</t>
+  </si>
+  <si>
+    <t>VTech DECT 6.0 Four Handset Cordless Phones with ITAD, CID, Backlit Keypads and Screens, Full Duplex Handset Speakerphones, Call Block Silver/Black, CS6929-4</t>
+  </si>
+  <si>
+    <t>Panasonic KXTGF872CB 2-in-1 Corded/Cordless Phone, 2 Handsets, Black</t>
+  </si>
+  <si>
+    <t>AT&amp;T DL72219 DECT 6.0 2-Handset Cordless Phone for Home with Connect to Cell, Call Blocking, 1.8" Backlit Screen, Big Buttons, intercom, and Unsurpassed Range</t>
+  </si>
+  <si>
+    <t>Panasonic DECT 6.0 Expandable Cordless Phone with Answering Machine and Smart Call Block - 2 Cordless Handsets - KX-TGD532W (White)</t>
+  </si>
+  <si>
+    <t>Vtech Dect 6.0 2-Handset Cordless Phone System with Caller ID, Backlit Keypad and Screen(CS6114-21), Black</t>
+  </si>
+  <si>
+    <t>VTech DS6161 Dect_6.0 1-Handset Landline Telephone,Yellow</t>
+  </si>
+  <si>
+    <t>AT&amp;T CL82257 DECT 6.0 2-Handset Cordless Phone for Home with Answering Machine, Call Blocking, Caller ID Announcer, Intercom and Long Range, Rose Gold</t>
+  </si>
+  <si>
+    <t>VTech CS6919-25 Dect 6.0 2 Handset Landline Telephone, Metallic Blue</t>
+  </si>
+  <si>
+    <t>UMIDIGI A9 Cell Phone, 64GB Fully Unlocked Smartphone, 5150mAh Battery Android Phone with 6.53" HD+ Full Screen and 13MP AI Triple Camera (Granite Grey)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A31-128GB / 4GB - A315G/DSL Unlocked Dual Sim Phone w/Quad Camera 48MP+8MP+5MP+5MP GSM International Version (Prism Crush Black)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy J2 16 GB Black 5" Unlocked Phone 4G LTE</t>
+  </si>
+  <si>
+    <t>VTech DECT 6.0 Three Handset Cordless Phone with CID, Backlit Keypads and Screens, Full Duplex Handset Speakerphones, Call Block Silver/Black</t>
+  </si>
+  <si>
+    <t>VTech DECT 6.0 Dual Handset Cordless Phones with CID, Backlit Keypads and Screens, Full Duplex Handset Speakerphones, and Call Block Silver/Black</t>
+  </si>
+  <si>
+    <t>Panasonic KXTGC382B Dect_6.0 2-Handset Landline Telephone</t>
+  </si>
+  <si>
+    <t>Panasonic KXTGD392B Dect_6.0 2-Handset Landline Telephone</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A11 32GB (6.4 inch) Display Triple Camera A115U Black Unlocked Smartphone (Renewed)</t>
+  </si>
+  <si>
+    <t>LG Phoenix 5 LM-K300AM 5.7" HD 16GB Unlocked 4G LTE Smartphone (AT&amp;T Packaging)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A32 4G Volte Unlocked 128GB Quad Camera - LTE Latin 6.4" Screen - International Version - SM-A325M/DS (Black, 128GB)</t>
+  </si>
+  <si>
+    <t>Phone Holder for Car, Car Phone Holder, Long Arm Dashboard Windshield Car Phone Mount, Strong Sticky Gel Suction Cup, Compatible iPhone 12/11 pro/11 pro max/XS/XR/X/8/7,Galaxy and More</t>
+  </si>
+  <si>
+    <t>Motorola ML1100 DECT 6.0 Expandable 4-line Business Phone System with Voicemail, Digital Receptionist and Music on Hold, Black</t>
+  </si>
+  <si>
+    <t>OCASE Samsung Galaxy S20 FE Case, Premium PU Leather S20 FE Phone case [TPU Inner Shell][RFID Blocking][Card Holder] Flip Wallet Cover Compatible with Samsung Galaxy S20FE 6.5 Inch-Blue</t>
+  </si>
+  <si>
+    <t>OCASE iPhone 11 Case, Premium PU Leather iPhone 11 case [TPU Inner Shell][Kickstand][Card Holder] Flip Wallet Phone Cover - for The 6.1 inch iPhone 11 -Black</t>
+  </si>
+  <si>
+    <t>UMIDIGI Smart Watch, Built-in GPS Fitness Tracker, Heart Rate Monitor Activity Tracker with 1.3" Touch Screen, 5ATM Waterproof Smartwatch for Men and Women, Compatible with iPhone and Android Phone.</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A12 SM-A125F Dual-SIM 128GB ROM + 4GB RAM Factory Unlocked 4G/LTE Smartphone (Blue) - International Version</t>
+  </si>
+  <si>
+    <t>Panasonic KXTGC384B Dect_6.0 4-Handset Landline Telephone</t>
+  </si>
+  <si>
+    <t>VTech IS8151-5 Super Long Range 5 Handset DECT 6.0 Cordless Phone for Home with Answering Machine, 2300 ft Range, Call Blocking, Bluetooth, Headset Jack, Power Backup, Intercom, Expandable to 12 HS</t>
+  </si>
+  <si>
+    <t>UMIDIGI A7S Unlocked Cell Phones(2GB+32GB), 6.53" HD+ Full Screen, 4150mAh Battery Smartphone with 13MP Ultra Wide Triple Camera, Dual 4G Volte (Sky Blue)</t>
+  </si>
+  <si>
+    <t>Uleway 3G Unlocked Basic Cell Phone Big Icon Unlocked Feature Phone with FM Radio LED Torch Easy to Use Mobile Phone fors Kids, as Backup Phone (Rogers, Telus, Bell)</t>
+  </si>
+  <si>
+    <t>Asus ROG Phone 5 ZS673KS / I005DA, 5G, International Version (No Warranty), Dual 128GB 12GB RAM, Tencent Games with Google Play, White - GSM Unlocked</t>
+  </si>
+  <si>
+    <t>OnePlus Nord N100 (64GB, 4GB) 6.52" 90Hz Display, Snapdragon, 5000mAh, Dual SIM GSM Factory Unlocked (Telus, Fido, Rogers, Global) International Model (Midnight Frost, 64GB SD Bundle)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A51 (SM-A515F/DS) Dual SIM 128GB,4GB RAM GSM Factory Unlocked (Blue)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A21S SM-A217M/DS (Black)</t>
+  </si>
+  <si>
+    <t>Easyfone Prime-A1 3G Unlocked GSM Senior Flip Cell Phone, Big Button Hearing Aids Compatible Easy-to-Use Basic Cell Phone with Charging Dock(Black)</t>
+  </si>
+  <si>
+    <t>Tryone Gooseneck Bed Phone Holder - Phone Mount Stand with 35in Flexible Lazy Long Arm for Desk Headboard Nightstand, Upgrade Large Clamp Compatible with iPhone 12 Mini 11 Pro Xs Max XR X 8 7 6 Plus</t>
+  </si>
+  <si>
+    <t>Android Phone, Blackview A80, 4G Dual sim Unlocked Cell Phones, Bundle Android 10 OS 2GB+16GB ROM Unlocked Smartphones, 6.21" HD+, Fingerprint Face Detection, 4200mAh Capacity Battery Unlocked Phone</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A21s Dual-SIM SM-A217F/DS 32GB Factory Unlocked 4G/LTE Smartphone - International Version (Black)</t>
+  </si>
+  <si>
+    <t>Unlocked Smartphone, Ulefone Note 8 Quad-core 2GB+16GB Expansion 128GB Android Phone Unlocked, 5.5 inch Screen 5MP Triple Camera, 2700mAh Battery Dual SIM 3G Unlocked Cell Phone for Canada -Black</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A10S A107M 32GB Unlocked GSM DUOS Phone w/ Dual 13MP/2MP Camera (International Variant/US Compatible LTE)</t>
+  </si>
+  <si>
+    <t>Vtech DECT 6.0 3 Cordless Phones with Caller ID, ITAD, Black - CS6124-31</t>
+  </si>
+  <si>
+    <t>AT&amp;T Corded Phone with 25 min Digital Answering Machine, Backlit Tilt Display, Audio Assist, Speakerphone (CL4940BK), Black</t>
+  </si>
+  <si>
+    <t>Realme 7 (64GB, 6GB RAM) 6.5" 90Hz Display, 5000mAh Battery, 48MP Quad Camera, Global 4G LTE GSM Factory Unlocked, International Model - RMX2155 (Mist Blue)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S9 Unlocked 64GB Midnight Black Canadian Version G960W Smartphone (Renewed)</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A10e (Renewed)</t>
+  </si>
+  <si>
+    <t>Panasonic KXTGF870B 2-in-1 Corded/Cordless Phone, 1 Handset, Black</t>
+  </si>
+  <si>
+    <t>VTech DECT 6.0 Dual Handset Cordless Phones with ITAD, CID, Backlit Keypads and Screens, Full Duplex Handset Speakerphones, Call Block Red - CS6929-26</t>
+  </si>
+  <si>
+    <t>UMIDIGI A11 Cell Phone, (4+128GB) 6.53" HD+ Full Screen Unlocked Smartphone, 5150mAh Battery Android Phone with Dual SIM (Global 4G LTE) Android 11 (Frost Grey, 4+128G)</t>
+  </si>
+  <si>
+    <t>Jethro [SC490] 4G/LTE Unlocked Bar Style Cell Phone for Seniors &amp; Kids, Big Screen and Large Buttons, Hearing Aid Compatible with Charging Dock, FCC &amp; IC Certified.</t>
+  </si>
+  <si>
+    <t>Panasonic KXTGD593W Dect_6.0 3-Handset Landline Telephone</t>
+  </si>
+  <si>
+    <t>Ushining 3G Feature Phone Big Icon Unlocked Basic Cell Phone with LED Torch Easy to Use Mobile Phone for Kids Seniors</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy A32 (5G) 64GB 6.5" Display Quad Camera Long Lasting Battery A326U Factory Unlocked Smartphone - Aura Black (Renewed)</t>
+  </si>
+  <si>
+    <t>Unlocked Cell Phone,Ulefone Note 11P Android 11 Smartphone 8GB +128GB 4G-LTE Unlocked Phone Global Vision 4400mAh 48MP Camera 6.55" Mobile Phone-Black</t>
+  </si>
+  <si>
+    <t>FLOVEME Magnetic Cell Phone Holder for Car Hands Free Phone Mount Compatible with iPhone 12 11 Pro Max XR XS 8 7 Plus Samsung Galaxy S10 S9 S8 Car Dashboard Magnet Phone Holder</t>
+  </si>
+  <si>
+    <t>Samsung A11 (32GB, A11, Blue)</t>
+  </si>
+  <si>
+    <t>Cell Phone UV Sanitizer, Newild Smart Sterilizer 1 Pro, 2nd Generation Non-Mercury UV, LED UV Light Cleaner Box with Aromatherapy Function, Disinfector for Mobile Phone Toothbrush Keys Jewelry Watch</t>
+  </si>
+  <si>
+    <t>Cell Phone Stand (Black, Non-Foldable)</t>
+  </si>
+  <si>
+    <t>Flian Smart Watch for Android iOS Phones, Fitness Tracker 1.69inch Touch Screen Smartwatch for Women Men Sleep and Heart Rate Monitor, Step Counter, Waterproof Fitness Watch Wristband, Montre intelligente pour Femmes Hommes</t>
   </si>
   <si>
     <t>earbuds</t>
+  </si>
+  <si>
+    <t>phones</t>
   </si>
 </sst>
 </file>
@@ -615,7 +792,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -637,10 +814,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -648,10 +825,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -659,10 +836,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -670,10 +847,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -681,10 +858,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -692,10 +869,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -703,329 +880,329 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>22</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B22">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>69</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>174</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>159</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>101</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>31</v>
+        <v>249</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1033,10 +1210,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1044,10 +1221,10 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>249</v>
+        <v>119</v>
       </c>
       <c r="C39" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1058,7 +1235,7 @@
         <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1066,10 +1243,10 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>179</v>
+        <v>29</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1077,10 +1254,10 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>299</v>
+        <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1088,10 +1265,10 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1099,10 +1276,10 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1113,7 +1290,7 @@
         <v>149</v>
       </c>
       <c r="C45" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1121,10 +1298,10 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1132,10 +1309,10 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1143,65 +1320,65 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B49">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B51">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B52">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C52" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B53">
-        <v>22</v>
+        <v>197</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1209,10 +1386,10 @@
         <v>51</v>
       </c>
       <c r="B54">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1223,7 +1400,7 @@
         <v>29</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1231,43 +1408,43 @@
         <v>53</v>
       </c>
       <c r="B56">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B57">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B58">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B59">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1275,54 +1452,54 @@
         <v>56</v>
       </c>
       <c r="B60">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B61">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B62">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C62" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B63">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C63" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B64">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="C64" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1330,10 +1507,10 @@
         <v>60</v>
       </c>
       <c r="B65">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C65" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1341,10 +1518,10 @@
         <v>61</v>
       </c>
       <c r="B66">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C66" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1352,10 +1529,10 @@
         <v>62</v>
       </c>
       <c r="B67">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="C67" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1363,10 +1540,10 @@
         <v>63</v>
       </c>
       <c r="B68">
-        <v>64</v>
+        <v>199</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1374,10 +1551,10 @@
         <v>64</v>
       </c>
       <c r="B69">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1385,10 +1562,681 @@
         <v>65</v>
       </c>
       <c r="B70">
-        <v>18</v>
+        <v>269</v>
       </c>
       <c r="C70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
         <v>66</v>
+      </c>
+      <c r="B71">
+        <v>199</v>
+      </c>
+      <c r="C71" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72">
+        <v>182</v>
+      </c>
+      <c r="C72" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>68</v>
+      </c>
+      <c r="B73">
+        <v>99</v>
+      </c>
+      <c r="C73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>69</v>
+      </c>
+      <c r="B74">
+        <v>120</v>
+      </c>
+      <c r="C74" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75">
+        <v>73</v>
+      </c>
+      <c r="C75" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76">
+        <v>76</v>
+      </c>
+      <c r="C76" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77">
+        <v>32</v>
+      </c>
+      <c r="C77" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B78">
+        <v>51</v>
+      </c>
+      <c r="C78" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79">
+        <v>86</v>
+      </c>
+      <c r="C79" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>75</v>
+      </c>
+      <c r="B80">
+        <v>49</v>
+      </c>
+      <c r="C80" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>76</v>
+      </c>
+      <c r="B81">
+        <v>84</v>
+      </c>
+      <c r="C81" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>77</v>
+      </c>
+      <c r="B82">
+        <v>199</v>
+      </c>
+      <c r="C82" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>78</v>
+      </c>
+      <c r="B83">
+        <v>349</v>
+      </c>
+      <c r="C83" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84">
+        <v>116</v>
+      </c>
+      <c r="C84" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85">
+        <v>69</v>
+      </c>
+      <c r="C85" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>72</v>
+      </c>
+      <c r="B86">
+        <v>49</v>
+      </c>
+      <c r="C86" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>64</v>
+      </c>
+      <c r="B87">
+        <v>32</v>
+      </c>
+      <c r="C87" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>81</v>
+      </c>
+      <c r="B88">
+        <v>128</v>
+      </c>
+      <c r="C88" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>82</v>
+      </c>
+      <c r="B89">
+        <v>70</v>
+      </c>
+      <c r="C89" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>83</v>
+      </c>
+      <c r="B90">
+        <v>79</v>
+      </c>
+      <c r="C90" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>84</v>
+      </c>
+      <c r="B91">
+        <v>197</v>
+      </c>
+      <c r="C91" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92">
+        <v>112</v>
+      </c>
+      <c r="C92" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>86</v>
+      </c>
+      <c r="B93">
+        <v>338</v>
+      </c>
+      <c r="C93" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>87</v>
+      </c>
+      <c r="B94">
+        <v>17</v>
+      </c>
+      <c r="C94" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>88</v>
+      </c>
+      <c r="B95">
+        <v>139</v>
+      </c>
+      <c r="C95" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>89</v>
+      </c>
+      <c r="B96">
+        <v>23</v>
+      </c>
+      <c r="C96" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>90</v>
+      </c>
+      <c r="B97">
+        <v>25</v>
+      </c>
+      <c r="C97" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98">
+        <v>66</v>
+      </c>
+      <c r="C98" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>92</v>
+      </c>
+      <c r="B99">
+        <v>261</v>
+      </c>
+      <c r="C99" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>93</v>
+      </c>
+      <c r="B100">
+        <v>149</v>
+      </c>
+      <c r="C100" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>94</v>
+      </c>
+      <c r="B101">
+        <v>171</v>
+      </c>
+      <c r="C101" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>95</v>
+      </c>
+      <c r="B102">
+        <v>159</v>
+      </c>
+      <c r="C102" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>96</v>
+      </c>
+      <c r="B103">
+        <v>44</v>
+      </c>
+      <c r="C103" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>97</v>
+      </c>
+      <c r="B104">
+        <v>999</v>
+      </c>
+      <c r="C104" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>98</v>
+      </c>
+      <c r="B105">
+        <v>408</v>
+      </c>
+      <c r="C105" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>99</v>
+      </c>
+      <c r="B106">
+        <v>253</v>
+      </c>
+      <c r="C106" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>75</v>
+      </c>
+      <c r="B107">
+        <v>49</v>
+      </c>
+      <c r="C107" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>100</v>
+      </c>
+      <c r="B108">
+        <v>89</v>
+      </c>
+      <c r="C108" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>101</v>
+      </c>
+      <c r="B109">
+        <v>24</v>
+      </c>
+      <c r="C109" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>102</v>
+      </c>
+      <c r="B110">
+        <v>129</v>
+      </c>
+      <c r="C110" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>103</v>
+      </c>
+      <c r="B111">
+        <v>260</v>
+      </c>
+      <c r="C111" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>104</v>
+      </c>
+      <c r="B112">
+        <v>119</v>
+      </c>
+      <c r="C112" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>105</v>
+      </c>
+      <c r="B113">
+        <v>54</v>
+      </c>
+      <c r="C113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>106</v>
+      </c>
+      <c r="B114">
+        <v>49</v>
+      </c>
+      <c r="C114" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>107</v>
+      </c>
+      <c r="B115">
+        <v>279</v>
+      </c>
+      <c r="C115" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>108</v>
+      </c>
+      <c r="B116">
+        <v>299</v>
+      </c>
+      <c r="C116" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>109</v>
+      </c>
+      <c r="B117">
+        <v>155</v>
+      </c>
+      <c r="C117" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>110</v>
+      </c>
+      <c r="B118">
+        <v>108</v>
+      </c>
+      <c r="C118" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>111</v>
+      </c>
+      <c r="B119">
+        <v>47</v>
+      </c>
+      <c r="C119" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>112</v>
+      </c>
+      <c r="B120">
+        <v>249</v>
+      </c>
+      <c r="C120" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>113</v>
+      </c>
+      <c r="B121">
+        <v>124</v>
+      </c>
+      <c r="C121" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>114</v>
+      </c>
+      <c r="B122">
+        <v>150</v>
+      </c>
+      <c r="C122" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>115</v>
+      </c>
+      <c r="B123">
+        <v>45</v>
+      </c>
+      <c r="C123" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>116</v>
+      </c>
+      <c r="B124">
+        <v>279</v>
+      </c>
+      <c r="C124" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>117</v>
+      </c>
+      <c r="B125">
+        <v>17</v>
+      </c>
+      <c r="C125" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>118</v>
+      </c>
+      <c r="B126">
+        <v>197</v>
+      </c>
+      <c r="C126" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>119</v>
+      </c>
+      <c r="B127">
+        <v>54</v>
+      </c>
+      <c r="C127" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>120</v>
+      </c>
+      <c r="B128">
+        <v>9</v>
+      </c>
+      <c r="C128" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>121</v>
+      </c>
+      <c r="B129">
+        <v>56</v>
+      </c>
+      <c r="C129" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>122</v>
+      </c>
+      <c r="B130">
+        <v>22</v>
+      </c>
+      <c r="C130" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>123</v>
+      </c>
+      <c r="B131">
+        <v>67</v>
+      </c>
+      <c r="C131" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addign text to projects.html
</commit_message>
<xml_diff>
--- a/Website/static/amazon/Amazon Web-Scraper.xlsx
+++ b/Website/static/amazon/Amazon Web-Scraper.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="119">
   <si>
     <t>Name</t>
   </si>
@@ -25,373 +25,352 @@
     <t>Search Term</t>
   </si>
   <si>
+    <t>Apple AirPods with Charging Case</t>
+  </si>
+  <si>
     <t>Wireless Earbuds, UMIDIGI AirBuds U Wireless Headphones with Microphones, Bluetooth 5.1 Earphones in-Ear, Touch Control Bluetooth Earbuds, 24H Playing Time for Work and Home Office.</t>
   </si>
   <si>
+    <t>Apple AirPods Pro</t>
+  </si>
+  <si>
     <t>Truly Wireless Earbuds, Tronsmart Noise Cancelling Earbuds with Charging Case, Built-in Clear Call Mics, Hi-Fi Stereo Audio Bluetooth Headphones, Sensitive Touch &amp; Waterproof Earphones for Sports Gaming Work Travel</t>
   </si>
   <si>
+    <t>Wireless Earbuds Bluetooth 5.0 Headphones,40H Playtime w/Wireless Charging Case,IP6 Waterproof/Button Control/TWS Stereo Bluetooth Earphones in-Ear w/Mic for Running Workout Gym</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Tribit 100H Playtime Bluetooth 5.0 IPX8 Waterproof Touch Control Ture Wireless Bluetooth Earbuds with Mic Earphone in-Ear Deep Bass Built-in Mic Bluetooth Headphones, Flybuds 3</t>
+  </si>
+  <si>
+    <t>Hi-Res Extra Bass Earbuds Noise Isolating in-Ear Headphones Wired Earbuds with Microphone for iPhone, iPod, iPad, MP3, Huawei, Samsung, Lightweight Earphones with Volume Control 3.5mm Jack Headphones</t>
+  </si>
+  <si>
+    <t>Apple EarPods with Lightning Connector</t>
+  </si>
+  <si>
+    <t>Sony MDRZX110 Over-Ear Headphones (Black)</t>
+  </si>
+  <si>
+    <t>Sony MDREX15LP/B In-Ear Headphones (Black)</t>
+  </si>
+  <si>
+    <t>Panasonic RPHJE120K In-Ear Headphone, Black</t>
+  </si>
+  <si>
+    <t>Sennheiser CX 80S in-Ear Headphones with in-line One-Button Smart Remote – Black</t>
+  </si>
+  <si>
+    <t>Monster Wireless Earbuds,Super Fast Charge,Bluetooth 5.0 in-Ear Stereo Headphones with USB-C Charging Case,Built-in Mic for Clear Calls,Water Resistant Design for Sports,Black.</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds,AXLOIE Active Noise Cancelling Bluetooth Earphones,in-Ear Wireless Headphones with 4-Mic Clear Call,ANC Stereo Earbuds Premium Deep Bass,with Portable Charging Case,19H Playtime</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Bluetooth Earbuds Bass+ Stereo Sound/USB-C Fast Charging/28H Playtime/IPX7 Waterproof Wireless Earphones Sport Headphones in Ear Bluetooth Earphones with Mic for Workout Gym (Black)</t>
+  </si>
+  <si>
+    <t>Wireless Bluetooth 5.0 Earbuds Headset in-Ear Noise Canceling Sport Headphones with LED Digital Shows Charging Case,Stereo Touch Control Waterproof Earphones Built-in Mic for Workout/Running/Gym (Black)</t>
+  </si>
+  <si>
     <t>Skullcandy Dime True Wireless Earbuds, True Black (S2DMW-P740)</t>
   </si>
   <si>
+    <t>Monster Wireless Earbuds, Bluetooth 5.0 in-Ear Stereo Headphones, Built-in Mics for Clear Calls, USB-C Quick Charge, 24-Hour Playtime, Single/Twin Mode for iPhone/Android</t>
+  </si>
+  <si>
+    <t>OKIMO Wireless Earbuds Bluetooth 5 Headphones with 3500mAh LED Charging Case, IPX7 Waterproof TWS Stereo Earphones in Ear, Hands-Free Headset with Mic, Touch Control, 125 Hours Playback for for Work / Home Office (Black)</t>
+  </si>
+  <si>
+    <t>Wireless Bluetooth earbuds, Bluetooth 5.0 in-ear headphones, 6D stereo IPX5 sweatproof, clear binaural call microphone, fitness, entertainment time charging box, noise reduction mini earbuds, sweatproof for mobile phones and Android Gym Sport（Black）</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, AIKELA Bluetooth 5.1 Earbuds Waterproof Touch Control Wireless Earphones with Hi-Fi Stereo Audio, Type-C Quick Charging Case, 15H Playtime, Single/Twin Mode, Built-in Mic for Gym, Home, Office</t>
+  </si>
+  <si>
+    <t>Apple EarPods with 3.5mm Headphone Plug</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Buds Live (Black) - True Wireless, Active Noise Cancelling, Wireless Charging Case (CAD Version)</t>
+  </si>
+  <si>
+    <t>Upgraded Tranya T10 Wireless Earbuds, 12mm Driver with Premium Deep Bass, Low Latency Game Mode, IPX7 Waterproof, Bluetooth 5.0 in Ear Headphones and Fast Charging</t>
+  </si>
+  <si>
+    <t>Apple AirPods with Wireless Charging Case</t>
+  </si>
+  <si>
+    <t>Monster Mission V1 Wireless Earbuds, Bluetooth 5.0 Built-in Mic Noise Cancelling Gaming Earbuds, Cool Light Effects with Music &amp; Game Modes, 48ms Ultra Low-Latency Gaming Earphones (Black) (Gray)</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Bluetooth Earbuds in Ear w/Wireless Charging Case/USB-C, 30H Playtime, Punchy Bass Sound Wireless Earphones, IPX7 Wireless Headphones w/Mic/Precise Button/Mono Mode</t>
+  </si>
+  <si>
+    <t>Skullcandy Jib Earbuds with Microphone, Purple (S2DUYK-629)</t>
+  </si>
+  <si>
+    <t>Monster Wireless Earbuds, Bluetooth 5.0 in-Ear Headphones with Charging Case, Stereo Earphones Deep Bass Sound, IPX5 Waterproof, Built-in Mic, Clear Call, Secure Fit for Sports</t>
+  </si>
+  <si>
+    <t>Sony MDR-XB50AP/B Extra Bass Earbud Headphones (Black)</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Bluetooth Earbuds with CVC8.0 Noise Cancelling Mics, 35H Playtime/Deep Bass/USB-C Quick Charge/Touch Control, IPX8 Waterproof Headphones for Work Sport</t>
+  </si>
+  <si>
+    <t>Anker Soundcore Life P2 True Wireless Earbuds with 4 Microphones,CVC 8.0 Noise Reduction, Graphene Driver, Clear Sound, USB C, 40H Playtime, IPX7 Waterproof, Wireless Earphones for Work, Home Office</t>
+  </si>
+  <si>
+    <t>JUKSTG Earphones Noise Isolating in-Ear Headphones with Pure Sound and Powerful Bass with High Sensitivity Microphone and Volume Control</t>
+  </si>
+  <si>
+    <t>True Wireless Earbuds, Bluetooth 5.0 in-Ear Headphones with Charging Box, IPX7 Waterproof Stereo Headphones in-Ear Earphones, Headset Built in Mic, Premium Sound with Deep Bass, Sport/Work</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, MDots Bluetooth Earbuds Immersive Stereo Sound, Bluetooth Earphones Twin&amp;Mono Mode, Wireless Headphones in Ear with Microphones/Precise Button Control/IPX6 Waterproof for Sport</t>
+  </si>
+  <si>
+    <t>ULIX Rider Earphones in-Ear Headphones with Mic, 3 Years Warranty, with Anti-Tangle, Braided Cable, Microphone, Super Resistant, 48 Ω Driver, Intense Bass, Earbuds for Samsung, Computer, Laptop</t>
+  </si>
+  <si>
+    <t>Vipcall Wireless Earbuds, in-Ear Bluetooth Headphones, Immersive Bass Sound, IPX8 Waterproof Sport Earphones, Touch Control Bluetooth Earbuds, 25 Hrs w/USB-C Charging Case/Twin&amp;Mono Mode/Mics, Black</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds Active Noise Cancellation, Bluetooth Earbuds 32 Hours Cycle Playtime with Type-C Charging Case Smart Touch ANC Wireless Earphones, Built-in 4Mics Bluetooth V5.0 Headsets Stereo Call, Deep Bass Sound A9 Wireless Headphones with IPX7 Waterproof for Outdoor Sport</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, 48Hours Playtime True Wireless Bluetooth Earbuds Noise Reduction Stereo Call Built-in Mics Wireless Earphones Extra Bass Sound E90 Wireless Headphones Waterpoof IPX8 Bluetooth V5.0 Headsets with Type-C Port Charging Case</t>
+  </si>
+  <si>
+    <t>Wireless Bluetooth Earbuds, AIKELA Active Noise Cancelling Ear Buds with 4 Mics, Activate Voice Assistant, Hi-FI Stereo Sound in-Ear Headphones with Wireless Charging Box, Touch Control Bluetooth 5.0 Sport Earphones Support 3 Play Modes</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, EarFun Air 4 Mics Noise Canceling, Bluetooth 5.0 Earbuds Touch Control, Wireless Charging, USB-C Quick Charge, Deep Bass, in-Ear Detection Headphones, 35H Playtime, IPX7 Waterproof</t>
+  </si>
+  <si>
+    <t>GO5 Mini Wireless Earbuds Bluetooth Headphones Premium Fidelity Sound Quality Wireless Charging Case Digital LED Intelligence Display IPX7 Waterproof Earphones Built-in Mic Headset for Sport Black</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy Buds Pro - Black</t>
+  </si>
+  <si>
+    <t>Bluetooth Earbuds, Wireless Earbuds Pink, Deep Bass Bluetooth Earphones w/Ergonomic Design/Mono&amp;Twin Mode/25 Hrs/IPX8 Waterproof/Microphones/Type-C Charging for Sport</t>
+  </si>
+  <si>
+    <t>Monster Mission V1 Wireless Earbuds, Bluetooth 5.0 Built-in Mic Noise Cancelling Gaming Earbuds, Cool Light Effects with Music &amp; Game Modes, 48ms Ultra Low-Latency Gaming Earphones (Black)</t>
+  </si>
+  <si>
+    <t>ULIX Rider Earphones in-Ear Headphones with Mic, 3 Years Warranty, with Anti-Tangle, Reinforced Cable, Microphone, Super Resistant, 48 Ω Driver, Intense Bass, Earbuds for Samsung, Computer, Laptop</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, MDots Bluetooth Earbuds Rhythm Stereo Sound Wireless Earphones in Ear w/20 Hrs Playtime, IPX6 Waterproof Sports Headphones with Mic Single/Twin Mode for Running, Workout</t>
+  </si>
+  <si>
+    <t>New Beats Studio Buds – True Wireless Noise Cancelling Earbuds – Compatible with Apple &amp; Android, Built-in Microphone, IPX4 Rating, Sweat Resistant Earphones, Class 1 Bluetooth Headphones - Black</t>
+  </si>
+  <si>
+    <t>APEKX Bluetooth Headphones True Wireless Earbuds with Charging Case IPX7 Waterproof TWS Stereo Sound Earphones Built-in Mic in-Ear Headsets Deep Bass for Sport Running Black</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds,Bluetooth 5.0 Earbuds with Mic,True Wireless Earbuds Sport with Ear Hooks,Sweatproof Workout Headphones with Charging Case/50H Playtime/One Button Control/Fitness/Sports/Gym/Exercise</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds SoundPEATS T2 Bluetooth Earphone Hybrid Active Noise Cancelling, ANC Earphones with Transparency Mode, Bluetooth 5.1 in-Ear Headphones, 30 Hours Playtime, USB-C Quick Charge, Stereo Sound, 12mm Driver</t>
+  </si>
+  <si>
+    <t>JBL Tune 125TWS True Wireless In-Ear Bluetooth Headphones with up to 32 Hours of Combined Music Playtime - Black</t>
+  </si>
+  <si>
+    <t>True Wireless Bluetooth 5.1 Earbuds in-Ears Smart Touch Control Earphone IPX7 Waterproof 20Hrs Playtime TWS Stereo Earbuds for Exercise</t>
+  </si>
+  <si>
+    <t>Wireless Earbuds, Sports Bluetooth 5.1 Wireless Headphones Earhooks Earphones, HiFi in-Ear Stereo Sound Noise Cancelling Earbuds Build-in Mic Deep Bass, 40H Playtime IPX7 Waterproof Headset for Sport</t>
+  </si>
+  <si>
+    <t>Skullcandy Ink'd+ Earbuds with Microphone, Black (S2IMY-M448)</t>
+  </si>
+  <si>
     <t>Wireless Earbuds, GOSCIEN Headphones Wireless Immersive Bass Sound Bluetooth 5.0 Headphones with Noise Cancellation Mic, IPX5 Waterproof Bluetooth Earphone with Charging Case for Work, Sports</t>
   </si>
   <si>
-    <t>Wireless Earbuds, Tribit 100H Playtime Bluetooth 5.0 IPX8 Waterproof Touch Control Ture Wireless Bluetooth Earbuds with Mic Earphone in-Ear Deep Bass Built-in Mic Bluetooth Headphones, Flybuds 3</t>
-  </si>
-  <si>
-    <t>Hi-Res Extra Bass Earbuds Noise Isolating in-Ear Headphones Wired Earbuds with Microphone for iPhone, iPod, iPad, MP3, Huawei, Samsung, Lightweight Earphones with Volume Control 3.5mm Jack Headphones</t>
-  </si>
-  <si>
-    <t>Wireless Bluetooth 5.0 Earbuds Headset in-Ear Noise Canceling Sport Headphones with LED Digital Shows Charging Case,Stereo Touch Control Waterproof Earphones Built-in Mic for Workout/Running/Gym (Black)</t>
-  </si>
-  <si>
-    <t>Apple EarPods with Lightning Connector</t>
-  </si>
-  <si>
-    <t>Sony MDRZX110 Over-Ear Headphones (Black)</t>
-  </si>
-  <si>
-    <t>Sony MDREX15LP/B In-Ear Headphones (Black)</t>
-  </si>
-  <si>
-    <t>Panasonic RPTCM125V ErgoFit In-Ear Earbud Headphones with Mic and Controller, Violet</t>
-  </si>
-  <si>
-    <t>Sennheiser CX 300S in Ear Headphone with One-Button Smart Remote - Black</t>
-  </si>
-  <si>
-    <t>Monster Wireless Earbuds,Super Fast Charge,Bluetooth 5.0 in-Ear Stereo Headphones with USB-C Charging Case,Built-in Mic for Clear Calls,Water Resistant Design for Sports,Black.</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds Bluetooth 5.0 Headphones,40H Playtime w/Wireless Charging Case,IP6 Waterproof/Button Control/TWS Stereo Bluetooth Earphones in-Ear w/Mic for Running Workout Gym</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, AIKELA Bluetooth 5.1 Earbuds Waterproof Touch Control Wireless Earphones with Hi-Fi Stereo Audio, Type-C Quick Charging Case, 15H Playtime, Single/Twin Mode, Built-in Mic for Gym, Home, Office</t>
-  </si>
-  <si>
-    <t>Wireless Bluetooth earbuds, Bluetooth 5.0 in-ear headphones, 6D stereo IPX5 sweatproof, clear binaural call microphone, fitness, entertainment time charging box, noise reduction mini earbuds, sweatproof for mobile phones and Android Gym Sport（Black）</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Bluetooth Earbuds Bass+ Stereo Sound/USB-C Fast Charging/28H Playtime/IPX7 Waterproof Wireless Earphones Sport Headphones in Ear Bluetooth Earphones with Mic for Workout Gym (Black)</t>
-  </si>
-  <si>
-    <t>OKIMO Wireless Earbuds Bluetooth 5 Headphones with 3500mAh LED Charging Case, IPX7 Waterproof TWS Stereo Earphones in Ear, Hands-Free Headset with Mic, Touch Control, 125 Hours Playback for for Work / Home Office (Black)</t>
-  </si>
-  <si>
-    <t>Monster Wireless Earbuds, Bluetooth 5.0 in-Ear Stereo Headphones, Built-in Mics for Clear Calls, USB-C Quick Charge, 24-Hour Playtime, Single/Twin Mode for iPhone/Android</t>
-  </si>
-  <si>
-    <t>Anker Soundcore Life P2 True Wireless Earbuds with 4 Microphones,CVC 8.0 Noise Reduction, Graphene Driver, Clear Sound, USB C, 40H Playtime, IPX7 Waterproof, Wireless Earphones for Work, Home Office</t>
-  </si>
-  <si>
-    <t>Vipcall Wireless Earbuds, in-Ear Bluetooth Headphones, Immersive Bass Sound, IPX8 Waterproof Sport Earphones, Touch Control Bluetooth Earbuds, 25 Hrs w/USB-C Charging Case/Twin&amp;Mono Mode/Mics, Black</t>
-  </si>
-  <si>
-    <t>Apple EarPods with 3.5mm Headphone Plug</t>
-  </si>
-  <si>
-    <t>Apple AirPods with Charging Case</t>
-  </si>
-  <si>
-    <t>Monster Mission V1 Wireless Earbuds, Bluetooth 5.0 Built-in Mic Noise Cancelling Gaming Earbuds, Cool Light Effects with Music &amp; Game Modes, 48ms Ultra Low-Latency Gaming Earphones (Black)</t>
-  </si>
-  <si>
-    <t>Otium Wireless Earbuds Bluetooth 5.0 Headphones with Digital Intelligence LED Display 3500 mAH Charging Case 135H Playtime Stereo Sound Headset IPX8 Waterproof Built-in Mic for Home Office</t>
+    <t>Wireless Earbuds SoundPEATS TrueAir2 Earphones Bluetooth V5.2 with 4 Mic, CVC Noise Cancellation for Clear Calls Headphones Qualcomm 3040, aptX Codec, USB C, 25 Hours Playtime</t>
+  </si>
+  <si>
+    <t>Skullcandy Dime True Wireless Earbuds, Dark Blue/Green (S2DMW-P750)</t>
   </si>
   <si>
     <t>Wireless Earbuds, Bluetooth 5.1 Wireless Headphones in-Ear Stereo Sports Bluetooth Earphones, Noise Cancelling Earbuds with Mic Deep Bass, IPX7 Waterproof, 40H Playtime Wireless Headset for Sports</t>
   </si>
   <si>
-    <t>Wireless Earbuds, 48Hours Playtime True Wireless Bluetooth Earbuds Noise Reduction Stereo Call Built-in Mics Wireless Earphones Extra Bass Sound E90 Wireless Headphones Waterpoof IPX8 Bluetooth V5.0 Headsets with Type-C Port Charging Case</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, MDots Bluetooth Earbuds Immersive Stereo Sound, Bluetooth Earphones Twin&amp;Mono Mode, Wireless Headphones in Ear with Microphones/Precise Button Control/IPX6 Waterproof for Sport</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds,AXLOIE Active Noise Cancelling Bluetooth Earphones,in-Ear Wireless Headphones with 4-Mic Clear Call,ANC Stereo Earbuds Premium Deep Bass,with Portable Charging Case,19H Playtime</t>
-  </si>
-  <si>
-    <t>Apple AirPods Pro</t>
-  </si>
-  <si>
-    <t>GO5 Mini Wireless Earbuds Bluetooth Headphones Premium Fidelity Sound Quality Wireless Charging Case Digital LED Intelligence Display IPX7 Waterproof Earphones Built-in Mic Headset for Sport Black</t>
-  </si>
-  <si>
-    <t>JBL Tune 125TWS True Wireless In-Ear Bluetooth Headphones with up to 32 Hours of Combined Music Playtime - Black</t>
-  </si>
-  <si>
-    <t>Sony MDR-XB50AP/B Extra Bass Earbud Headphones (Black)</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Bluetooth Earbuds with CVC8.0 Noise Cancelling Mics, 35H Playtime/Deep Bass/USB-C Quick Charge/Touch Control, IPX8 Waterproof Headphones for Work Sport</t>
-  </si>
-  <si>
-    <t>True Wireless Earbuds, Bluetooth 5.0 in-Ear Headphones with Charging Box, IPX7 Waterproof Stereo Headphones in-Ear Earphones, Headset Built in Mic, Premium Sound with Deep Bass, Sport/Work</t>
-  </si>
-  <si>
-    <t>JUKSTG Earphones Noise Isolating in-Ear Headphones with Pure Sound and Powerful Bass with High Sensitivity Microphone and Volume Control</t>
-  </si>
-  <si>
-    <t>ULIX Rider Earphones in-Ear Headphones with Mic, 3 Years Warranty, with Anti-Tangle, Braided Cable, Microphone, Super Resistant, 48 Ω Driver, Intense Bass, Earbuds for Samsung, Computer, Laptop</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Buds Live (Black) - True Wireless, Active Noise Cancelling, Wireless Charging Case (CAD Version)</t>
-  </si>
-  <si>
-    <t>Panasonic RPHJE120K In-Ear Headphone, Black</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds Bluetooth 5.0 Wireless Headphones in-Ear Stereo Noise Cancelling Bluetooth Earbuds with LED Charging Case IPX7 Waterproof Touch Control Headset Built-in Mic Earphones for Sport/Work (black)</t>
-  </si>
-  <si>
-    <t>Wireless Bluetooth Earbuds, AIKELA Active Noise Cancelling Ear Buds with 4 Mics, Activate Voice Assistant, Hi-FI Stereo Sound in-Ear Headphones with Wireless Charging Box, Touch Control Bluetooth 5.0 Sport Earphones Support 3 Play Modes</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, MDots Bluetooth Earbuds Rhythm Stereo Sound Wireless Earphones in Ear w/20 Hrs Playtime, IPX6 Waterproof Sports Headphones with Mic Single/Twin Mode for Running, Workout</t>
-  </si>
-  <si>
-    <t>Monster Wireless Earbuds, Bluetooth 5.0 in-Ear Headphones with Charging Case, Stereo Earphones Deep Bass Sound, IPX5 Waterproof, Built-in Mic, Clear Call, Secure Fit for Sports</t>
-  </si>
-  <si>
-    <t>New Beats Studio Buds – True Wireless Noise Cancelling Earbuds – Compatible with Apple &amp; Android, Built-in Microphone, IPX4 Rating, Sweat Resistant Earphones, Class 1 Bluetooth Headphones - Black</t>
-  </si>
-  <si>
-    <t>ULIX Rider Earphones in-Ear Headphones with Mic, 3 Years Warranty, with Anti-Tangle, Reinforced Cable, Microphone, Super Resistant, 48 Ω Driver, Intense Bass, Earbuds for Samsung, Computer, Laptop</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy Buds Pro - Black</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds Active Noise Cancellation, Bluetooth Earbuds 32 Hours Cycle Playtime with Type-C Charging Case Smart Touch ANC Wireless Earphones, Built-in 4Mics Bluetooth V5.0 Headsets Stereo Call, Deep Bass Sound A9 Wireless Headphones with IPX7 Waterproof for Outdoor Sport</t>
-  </si>
-  <si>
-    <t>Bluetooth Earbuds, Wireless Earbuds Pink, Deep Bass Bluetooth Earphones w/Ergonomic Design/Mono&amp;Twin Mode/25 Hrs/IPX8 Waterproof/Microphones/Type-C Charging for Sport</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds SoundPEATS T2 Bluetooth Earphone Hybrid Active Noise Cancelling, ANC Earphones with Transparency Mode, Bluetooth 5.1 in-Ear Headphones, 30 Hours Playtime, USB-C Quick Charge, Stereo Sound, 12mm Driver</t>
-  </si>
-  <si>
-    <t>MMK Wireless Earbuds with Mic and Wireless Charge, 5.1 Bluetooth Touch Contral, IPX8 Waterproof In-Ear Earphone with CVC 8.0 Noise Cancelling, Built-in TWS Stereo Headphones with Deep Bass for Sport/ Work</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds SoundPEATS TrueAir2 Earphones Bluetooth V5.2 with 4 Mic, CVC Noise Cancellation for Clear Calls Headphones Qualcomm 3040, aptX Codec, USB C, 25 Hours Playtime</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, Bluetooth 5.0 Earbuds Waterproof Wireless Earphones, with 35H Playtime, Hi-Fi Audio Deep Bass, Noise-Canceling Mic, in-Ear Ear Buds with Charging Case, Sensitive Touch Control Bluetooth Sport Earphones, for Samsung/iPhone/Android</t>
-  </si>
-  <si>
-    <t>iKanzi Wireless Earbuds Bluetooth 5 Headphones with Charging Case, IPX7 Waterproof TWS Stereo Earphones in Ear, Hands-Free Headset with Mic, Touch Control, USB-C Fast Charging, 25 Hours Playback for iPhone and Android (black)</t>
-  </si>
-  <si>
-    <t>True Wireless Earbuds, in-Ear Bluetooth Earbuds , with Fast Charging Case Noise Canceling 3D Stereo Headsets Touch Control Headphones, HD Stereo Deep Bass Built-in Mic Waterproof Gym Sports Earphones (Black)</t>
-  </si>
-  <si>
-    <t>2021 Wireless Earbuds, Tribit Qualcomm QCC3040 Bluetooth 5.2, 4 Mics CVC 8.0 Call Noise Reduction 50H Playtime Clear Calls Volume Control True Wireless Bluetooth Earbuds Earphones, FlyBuds C1</t>
-  </si>
-  <si>
-    <t>2 Pack Earbuds/Headphones/Earphones with 3.5mm Wired in Ear Headphone Plug(Built-in Microphone &amp; Volume Control) Compatible with iPhone,iPad,iPod,PC,MP3/4,Android -White</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, EarFun Air 4 Mics Noise Canceling, Bluetooth 5.0 Earbuds Touch Control, Wireless Charging, USB-C Quick Charge, Deep Bass, in-Ear Detection Headphones, 35H Playtime, IPX7 Waterproof</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds, 5.0 Bluetooth Earbuds,Touch Control Cute Cat Wireless Earset with Microphone - Hi-Fi Stereo Audio, Noise Reduction, Waterproof for iPhone/Android to Kids Adult Gift</t>
-  </si>
-  <si>
-    <t>42 Hours Wireless Earbuds, Forte Wireless Earphones Bluetooth 5.0 Premium Lossless Audio with Smooth Switch Stereo or Mono, Smart Touch Bluetooth Earbuds Built-in Mics Headset, Wireless Headphones IPX8 Type-C for Sport and Travel</t>
-  </si>
-  <si>
-    <t>Wireless Earbuds E19 Bluetooth Earbuds 15Hours Cycle Playtime with Mini Charging Case, 3D Stereo Sound Wireless Earphones Built-in Mic Headsets for Gym Sport, True Wireless Headphones for iOS and Android Bluetooth Device</t>
-  </si>
-  <si>
-    <t>UMIDIGI A9 Cell Phone, 64GB Fully Unlocked Smartphone, 5150mAh Battery Android Phone with 6.53" HD+ Full Screen and 13MP AI Triple Camera (Peacock Green)</t>
-  </si>
-  <si>
-    <t>Panasonic Dect_6.0 4-Handset Landline Telephone</t>
-  </si>
-  <si>
-    <t>UMIDIGI A9 Pro Unlocked Cell Phones 6.3" FHD+ Full Screen, 4150mAh High Capacity Battery Smartphone with AI Matrix Quad Camera, Dual SIM Phone (Forest Green, 6+128GB)</t>
-  </si>
-  <si>
-    <t>Motorola ML1000 DECT 6.0 Expandable 4-line Business Phone System with Voicemail, Digital Receptionist and Music on Hold, Black</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A10e 32GB Unlocked Phone - Black</t>
-  </si>
-  <si>
-    <t>VTech DECT 6.0 Four Handset Cordless Phones with ITAD, CID, Backlit Keypads and Screens, Full Duplex Handset Speakerphones, Call Block Silver/Black, CS6929-4</t>
-  </si>
-  <si>
-    <t>Panasonic KXTGF872CB 2-in-1 Corded/Cordless Phone, 2 Handsets, Black</t>
-  </si>
-  <si>
-    <t>AT&amp;T DL72219 DECT 6.0 2-Handset Cordless Phone for Home with Connect to Cell, Call Blocking, 1.8" Backlit Screen, Big Buttons, intercom, and Unsurpassed Range</t>
-  </si>
-  <si>
-    <t>Panasonic DECT 6.0 Expandable Cordless Phone with Answering Machine and Smart Call Block - 2 Cordless Handsets - KX-TGD532W (White)</t>
-  </si>
-  <si>
-    <t>Vtech Dect 6.0 2-Handset Cordless Phone System with Caller ID, Backlit Keypad and Screen(CS6114-21), Black</t>
-  </si>
-  <si>
-    <t>VTech DS6161 Dect_6.0 1-Handset Landline Telephone,Yellow</t>
-  </si>
-  <si>
-    <t>AT&amp;T CL82257 DECT 6.0 2-Handset Cordless Phone for Home with Answering Machine, Call Blocking, Caller ID Announcer, Intercom and Long Range, Rose Gold</t>
-  </si>
-  <si>
-    <t>VTech CS6919-25 Dect 6.0 2 Handset Landline Telephone, Metallic Blue</t>
-  </si>
-  <si>
-    <t>UMIDIGI A9 Cell Phone, 64GB Fully Unlocked Smartphone, 5150mAh Battery Android Phone with 6.53" HD+ Full Screen and 13MP AI Triple Camera (Granite Grey)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A31-128GB / 4GB - A315G/DSL Unlocked Dual Sim Phone w/Quad Camera 48MP+8MP+5MP+5MP GSM International Version (Prism Crush Black)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy J2 16 GB Black 5" Unlocked Phone 4G LTE</t>
-  </si>
-  <si>
-    <t>VTech DECT 6.0 Three Handset Cordless Phone with CID, Backlit Keypads and Screens, Full Duplex Handset Speakerphones, Call Block Silver/Black</t>
-  </si>
-  <si>
-    <t>VTech DECT 6.0 Dual Handset Cordless Phones with CID, Backlit Keypads and Screens, Full Duplex Handset Speakerphones, and Call Block Silver/Black</t>
-  </si>
-  <si>
-    <t>Panasonic KXTGC382B Dect_6.0 2-Handset Landline Telephone</t>
-  </si>
-  <si>
-    <t>Panasonic KXTGD392B Dect_6.0 2-Handset Landline Telephone</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A11 32GB (6.4 inch) Display Triple Camera A115U Black Unlocked Smartphone (Renewed)</t>
-  </si>
-  <si>
-    <t>LG Phoenix 5 LM-K300AM 5.7" HD 16GB Unlocked 4G LTE Smartphone (AT&amp;T Packaging)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A32 4G Volte Unlocked 128GB Quad Camera - LTE Latin 6.4" Screen - International Version - SM-A325M/DS (Black, 128GB)</t>
-  </si>
-  <si>
-    <t>Phone Holder for Car, Car Phone Holder, Long Arm Dashboard Windshield Car Phone Mount, Strong Sticky Gel Suction Cup, Compatible iPhone 12/11 pro/11 pro max/XS/XR/X/8/7,Galaxy and More</t>
-  </si>
-  <si>
-    <t>Motorola ML1100 DECT 6.0 Expandable 4-line Business Phone System with Voicemail, Digital Receptionist and Music on Hold, Black</t>
-  </si>
-  <si>
-    <t>OCASE Samsung Galaxy S20 FE Case, Premium PU Leather S20 FE Phone case [TPU Inner Shell][RFID Blocking][Card Holder] Flip Wallet Cover Compatible with Samsung Galaxy S20FE 6.5 Inch-Blue</t>
-  </si>
-  <si>
-    <t>OCASE iPhone 11 Case, Premium PU Leather iPhone 11 case [TPU Inner Shell][Kickstand][Card Holder] Flip Wallet Phone Cover - for The 6.1 inch iPhone 11 -Black</t>
-  </si>
-  <si>
-    <t>UMIDIGI Smart Watch, Built-in GPS Fitness Tracker, Heart Rate Monitor Activity Tracker with 1.3" Touch Screen, 5ATM Waterproof Smartwatch for Men and Women, Compatible with iPhone and Android Phone.</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A12 SM-A125F Dual-SIM 128GB ROM + 4GB RAM Factory Unlocked 4G/LTE Smartphone (Blue) - International Version</t>
-  </si>
-  <si>
-    <t>Panasonic KXTGC384B Dect_6.0 4-Handset Landline Telephone</t>
-  </si>
-  <si>
-    <t>VTech IS8151-5 Super Long Range 5 Handset DECT 6.0 Cordless Phone for Home with Answering Machine, 2300 ft Range, Call Blocking, Bluetooth, Headset Jack, Power Backup, Intercom, Expandable to 12 HS</t>
-  </si>
-  <si>
-    <t>UMIDIGI A7S Unlocked Cell Phones(2GB+32GB), 6.53" HD+ Full Screen, 4150mAh Battery Smartphone with 13MP Ultra Wide Triple Camera, Dual 4G Volte (Sky Blue)</t>
-  </si>
-  <si>
-    <t>Uleway 3G Unlocked Basic Cell Phone Big Icon Unlocked Feature Phone with FM Radio LED Torch Easy to Use Mobile Phone fors Kids, as Backup Phone (Rogers, Telus, Bell)</t>
-  </si>
-  <si>
-    <t>Asus ROG Phone 5 ZS673KS / I005DA, 5G, International Version (No Warranty), Dual 128GB 12GB RAM, Tencent Games with Google Play, White - GSM Unlocked</t>
-  </si>
-  <si>
-    <t>OnePlus Nord N100 (64GB, 4GB) 6.52" 90Hz Display, Snapdragon, 5000mAh, Dual SIM GSM Factory Unlocked (Telus, Fido, Rogers, Global) International Model (Midnight Frost, 64GB SD Bundle)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A51 (SM-A515F/DS) Dual SIM 128GB,4GB RAM GSM Factory Unlocked (Blue)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A21S SM-A217M/DS (Black)</t>
-  </si>
-  <si>
-    <t>Easyfone Prime-A1 3G Unlocked GSM Senior Flip Cell Phone, Big Button Hearing Aids Compatible Easy-to-Use Basic Cell Phone with Charging Dock(Black)</t>
-  </si>
-  <si>
-    <t>Tryone Gooseneck Bed Phone Holder - Phone Mount Stand with 35in Flexible Lazy Long Arm for Desk Headboard Nightstand, Upgrade Large Clamp Compatible with iPhone 12 Mini 11 Pro Xs Max XR X 8 7 6 Plus</t>
-  </si>
-  <si>
-    <t>Android Phone, Blackview A80, 4G Dual sim Unlocked Cell Phones, Bundle Android 10 OS 2GB+16GB ROM Unlocked Smartphones, 6.21" HD+, Fingerprint Face Detection, 4200mAh Capacity Battery Unlocked Phone</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A21s Dual-SIM SM-A217F/DS 32GB Factory Unlocked 4G/LTE Smartphone - International Version (Black)</t>
-  </si>
-  <si>
-    <t>Unlocked Smartphone, Ulefone Note 8 Quad-core 2GB+16GB Expansion 128GB Android Phone Unlocked, 5.5 inch Screen 5MP Triple Camera, 2700mAh Battery Dual SIM 3G Unlocked Cell Phone for Canada -Black</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A10S A107M 32GB Unlocked GSM DUOS Phone w/ Dual 13MP/2MP Camera (International Variant/US Compatible LTE)</t>
-  </si>
-  <si>
-    <t>Vtech DECT 6.0 3 Cordless Phones with Caller ID, ITAD, Black - CS6124-31</t>
-  </si>
-  <si>
-    <t>AT&amp;T Corded Phone with 25 min Digital Answering Machine, Backlit Tilt Display, Audio Assist, Speakerphone (CL4940BK), Black</t>
-  </si>
-  <si>
-    <t>Realme 7 (64GB, 6GB RAM) 6.5" 90Hz Display, 5000mAh Battery, 48MP Quad Camera, Global 4G LTE GSM Factory Unlocked, International Model - RMX2155 (Mist Blue)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy S9 Unlocked 64GB Midnight Black Canadian Version G960W Smartphone (Renewed)</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A10e (Renewed)</t>
-  </si>
-  <si>
-    <t>Panasonic KXTGF870B 2-in-1 Corded/Cordless Phone, 1 Handset, Black</t>
-  </si>
-  <si>
-    <t>VTech DECT 6.0 Dual Handset Cordless Phones with ITAD, CID, Backlit Keypads and Screens, Full Duplex Handset Speakerphones, Call Block Red - CS6929-26</t>
-  </si>
-  <si>
-    <t>UMIDIGI A11 Cell Phone, (4+128GB) 6.53" HD+ Full Screen Unlocked Smartphone, 5150mAh Battery Android Phone with Dual SIM (Global 4G LTE) Android 11 (Frost Grey, 4+128G)</t>
-  </si>
-  <si>
-    <t>Jethro [SC490] 4G/LTE Unlocked Bar Style Cell Phone for Seniors &amp; Kids, Big Screen and Large Buttons, Hearing Aid Compatible with Charging Dock, FCC &amp; IC Certified.</t>
-  </si>
-  <si>
-    <t>Panasonic KXTGD593W Dect_6.0 3-Handset Landline Telephone</t>
-  </si>
-  <si>
-    <t>Ushining 3G Feature Phone Big Icon Unlocked Basic Cell Phone with LED Torch Easy to Use Mobile Phone for Kids Seniors</t>
-  </si>
-  <si>
-    <t>Samsung Galaxy A32 (5G) 64GB 6.5" Display Quad Camera Long Lasting Battery A326U Factory Unlocked Smartphone - Aura Black (Renewed)</t>
-  </si>
-  <si>
-    <t>Unlocked Cell Phone,Ulefone Note 11P Android 11 Smartphone 8GB +128GB 4G-LTE Unlocked Phone Global Vision 4400mAh 48MP Camera 6.55" Mobile Phone-Black</t>
-  </si>
-  <si>
-    <t>FLOVEME Magnetic Cell Phone Holder for Car Hands Free Phone Mount Compatible with iPhone 12 11 Pro Max XR XS 8 7 Plus Samsung Galaxy S10 S9 S8 Car Dashboard Magnet Phone Holder</t>
-  </si>
-  <si>
-    <t>Samsung A11 (32GB, A11, Blue)</t>
-  </si>
-  <si>
-    <t>Cell Phone UV Sanitizer, Newild Smart Sterilizer 1 Pro, 2nd Generation Non-Mercury UV, LED UV Light Cleaner Box with Aromatherapy Function, Disinfector for Mobile Phone Toothbrush Keys Jewelry Watch</t>
-  </si>
-  <si>
-    <t>Cell Phone Stand (Black, Non-Foldable)</t>
-  </si>
-  <si>
-    <t>Flian Smart Watch for Android iOS Phones, Fitness Tracker 1.69inch Touch Screen Smartwatch for Women Men Sleep and Heart Rate Monitor, Step Counter, Waterproof Fitness Watch Wristband, Montre intelligente pour Femmes Hommes</t>
+    <t>Wireless Earbuds, Apt-x Deep Bass Bluetooth Earbuds CVC8.0 Noise Reduction Stereo Call 8 Hours Continuous Playtime Bluetooth Earphones with Wireless Charging Portable Case Type-C, Black E60 IPX8 Waterproof Wireless Headphones Snug for Sport and Outdoor Travel Wireless Headsets</t>
+  </si>
+  <si>
+    <t>Caixun EC32S2N, 32‘’ Television 32 inch HD HDR Smart TV with Screen Share, HDMI, USB (2021 Model)</t>
+  </si>
+  <si>
+    <t>CtrlTV Remote for Sony Bravia Smart Remote and Sony Bravia UHD Crystal 4K Smart HDR OLED TVs LCD LED HDTV RMT-TX100U with Netflix XBR KDL Series</t>
+  </si>
+  <si>
+    <t>UNOCAR Replacement for Sony Smart Bravia Remote, Sony Bluetooth Voice Search Mic Remote and Sony Smart Bravia Android TVs, Sony 4K UHD Crystal HDR TV, Sony OLED Ultra HDTV, XBR KDL Series TV, RMF-TX300U</t>
+  </si>
+  <si>
+    <t>TCL 32" Class 3-Series HD LED Smart Android TV</t>
+  </si>
+  <si>
+    <t>TCL 65" Class 4-Series 4K UHD HDR Smart Roku TV - 65S435</t>
+  </si>
+  <si>
+    <t>Samsung 43" TU7000 4K Ultra HD HDR Smart TV (UN43TU7000FXZC) [Canada Version]</t>
+  </si>
+  <si>
+    <t>Samsung UN32M4500BFXZC 32" 720p HD Smart LED TV (2018), Black [Canada Version]</t>
+  </si>
+  <si>
+    <t>Samsung 55" TU8000 4K Ultra HD HDR Smart TV (UN55TU8000FXZC) [Canada Version]</t>
+  </si>
+  <si>
+    <t>Toshiba 50-inch 4K Ultra HD HDR Smart LED TV - Fire TV Edition Released 2020</t>
+  </si>
+  <si>
+    <t>Hisense 43A68G - 43" Smart TV Ultra HD 4K Dolby Vision HDR10 Android Television with Bluetooth, Voice Remote (Canada Model) (2021)</t>
+  </si>
+  <si>
+    <t>Samsung UN32N5300AFXZC 32" 1080p Full HD Smart LED TV (2018), Glossy Black [Canada Version]</t>
+  </si>
+  <si>
+    <t>Samsung 40" 1080p LED Smart TV (Black) (2019) (UN40N5200AFXZC) [Canada Version]</t>
+  </si>
+  <si>
+    <t>LG 24LJ4540 Electronics 24" 720p LED TV (2017 Model) - Black</t>
+  </si>
+  <si>
+    <t>Samsung - 43" Q60A QLED 4K Ultra HD HDR Smart TV [QN43Q60AAFXZC][Canada Version] (2021)</t>
+  </si>
+  <si>
+    <t>Caixun EC43S1A, 43 inch UHD HDR Smart Android TV with Google Assistant (Voice Control), Bluetooth,Wi-Fi,Chromecast Built-in, Screen Share, HDMI, USB (2021 Model)</t>
+  </si>
+  <si>
+    <t>Samsung 50" Q60T 4K Ultra HD HDR Smart QLED TV (QN50Q60TAFXZC) [Canada Version]</t>
+  </si>
+  <si>
+    <t>TCL 40S325-CA 1080p Smart LED Television (2019), 40"</t>
+  </si>
+  <si>
+    <t>TCL 32S327-CA 1080p Smart LED Television (2019), 32"</t>
+  </si>
+  <si>
+    <t>TCL 43" Class 4-Series 4K UHD HDR Smart Android TV - 43S434-CA</t>
+  </si>
+  <si>
+    <t>Mini Projector, [2021 Upgraded] 6000 Lumen Video Projector, 1080P Supported 210" Display, Compatible with Phone,Computer,Laptop,USB,HDMI,VGA</t>
+  </si>
+  <si>
+    <t>SIMOLIO Digital Wireless Headphones for TV, Hearing Protection Wireless TV Headphone W/Protein Earmuffs, Wireless TV Headset System for All TVs, TV Hearing Aid Device for Seniors and Hard of Hearing</t>
+  </si>
+  <si>
+    <t>Seagate IronWolf 12TB NAS Internal Hard Drive HDD – 3.5 Inch SATA 6Gb/s 7200 RPM 256MB Cache for RAID Network Attached Storage – Frustration Free Packaging (ST12000VN0008)</t>
+  </si>
+  <si>
+    <t>SANSUI ES32S1N 32" HD HDR Smart TV Television 32-inch Built-in HDMI, USB - Support Screen Cast Mirroring(2021 Model)</t>
+  </si>
+  <si>
+    <t>Samsung 55" LS03T The Frame 4K ULtra HD HDR Smart QLED TV (QN55LS03TAFXZC) [Canada Version]</t>
+  </si>
+  <si>
+    <t>Toshiba 32-inch 720p HD Smart LED TV - Fire TV Edition - Released 2020</t>
+  </si>
+  <si>
+    <t>Samsung 32" Q50AA QLED 4K Ultra HD HDR Smart TV [QN32Q50AAFXZ] [Canada Version] (2021)</t>
+  </si>
+  <si>
+    <t>LG 55UP7560 55" 4K UHD Smart TV</t>
+  </si>
+  <si>
+    <t>Samsung 43-inch TU-7000 Series Class Smart TV | Crystal UHD - 4K HDR - with Alexa Built-in | UN43TU7000FXZA, 2020 Model</t>
+  </si>
+  <si>
+    <t>Sony X80J 43 inch 4K Ultra HD HDR LED Smart Google TV with Dolby Vision (KD43X80J)</t>
+  </si>
+  <si>
+    <t>LG 49UN7300 49" 4K UHD Smart LED TV</t>
+  </si>
+  <si>
+    <t>Samsung - 50" AU8000 LED 4K Ultra HD HDR Smart TV [UN50AU8000FXZC][Canada Version] (2021)</t>
+  </si>
+  <si>
+    <t>LG 43UM6951 43" 4K UHD Smart LED TV, Black</t>
+  </si>
+  <si>
+    <t>Hisense 32H41G- 32 inch Smart Full Array LED Roku TV with DTS TruSurround, 3HDMI (Canada Model) 2021</t>
+  </si>
+  <si>
+    <t>Hisense 43A6GV - 43 inch Smart 4K Ultra HD VIDAA TV</t>
+  </si>
+  <si>
+    <t>Samsung - 32" Q60A QLED 4K Ultra HD HDR Smart TV [QN32Q60AAFXZC][Canada Version] (2021)</t>
+  </si>
+  <si>
+    <t>Hisense 40H55G - 40 inch Smart Full HD VIDAA TV</t>
+  </si>
+  <si>
+    <t>Samsung - 55" The Frame LED 4K UHD Smart TV [QN55LS03AAFXZC][Canada Version] (2021)</t>
+  </si>
+  <si>
+    <t>TCL 75" 5-Series 4K UHD Dolby Vision HDR QLED Roku Smart TV - 75S535-CA</t>
+  </si>
+  <si>
+    <t>LG OLED55C1 55" 4K Smart 120Hz OLED TV</t>
+  </si>
+  <si>
+    <t>Sony X85J 65 inch TV 4K Ultra HD HDR LED Smart Google TV with Dolby Vision &amp; Atmos (KD65X85J)</t>
+  </si>
+  <si>
+    <t>Samsung - 55" Q70A QLED 4K Ultra HD HDR Smart TV [QN55Q70AAFXZC][Canada Version] (2021)</t>
+  </si>
+  <si>
+    <t>Samsung - 50" QN90A QLED 4K Ultra HD HDR Smart TV [QN50QN90AAFXZC][Canada Version] (2021)</t>
+  </si>
+  <si>
+    <t>LG 55UP7700 55" 4K UHD Smart TV</t>
+  </si>
+  <si>
+    <t>Sony KDL32W600D 32-Inch 720P Smart LED Television</t>
+  </si>
+  <si>
+    <t>RCA RT1970 19&amp;quot; 720P LED HDTV</t>
+  </si>
+  <si>
+    <t>LG 75NANO80UNA Alexa Built-in Nano 8 Series 75" 4K Ultra HD Smart LED Nanocell TV (2020)</t>
+  </si>
+  <si>
+    <t>TCL 40" Class 3-Series HD LED Smart Android TV - 40S334-CA</t>
+  </si>
+  <si>
+    <t>LG 86UP8770 86" 4K/UHD 120Hz Smart TV</t>
+  </si>
+  <si>
+    <t>Sony X90J 55 inch BRAVIA XR Full Array LED 4K Ultra HD HDR Smart Google TV with Dolby Vision &amp; Atmos (XR55X90J)</t>
+  </si>
+  <si>
+    <t>Samsung - 85" QN85A QLED 4K Ultra HD HDR Smart TV [QN85QN85AAFXZC][Canada Version] (2021)</t>
+  </si>
+  <si>
+    <t>Samsung 50" TU8000 Crystal UHD 4K UHD Smart TV with Alexa Built-in UN50TU8000FXZA 2020</t>
+  </si>
+  <si>
+    <t>Samsung UN43N5300AFXZC 43" 1080p Full HD Smart LED TV (2018), Glossy Black [Canada Version]</t>
+  </si>
+  <si>
+    <t>Hisense 55" Smart TV Ultra HD 4K Dolby Vision HDR10 Android Television with 2.1 CH Sound Bar Speaker Built-in Subwoofer</t>
+  </si>
+  <si>
+    <t>LG 50NANO75 50" 4K Smart NanoCell TV</t>
   </si>
   <si>
     <t>earbuds</t>
   </si>
   <si>
-    <t>phones</t>
+    <t>tvs</t>
   </si>
 </sst>
 </file>
@@ -792,7 +771,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -814,10 +793,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>67</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -828,7 +807,7 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -836,10 +815,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>39</v>
+        <v>248</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -847,10 +826,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -858,10 +837,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -869,10 +848,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -880,21 +859,21 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -902,10 +881,10 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -913,10 +892,10 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -924,10 +903,10 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -935,10 +914,10 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -946,10 +925,10 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -957,10 +936,10 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -968,10 +947,10 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -979,10 +958,10 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -990,32 +969,32 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B19">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1023,76 +1002,76 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>99</v>
-      </c>
       <c r="C26" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B27">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1100,10 +1079,10 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>28</v>
+        <v>159</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1111,10 +1090,10 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1122,10 +1101,10 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>159</v>
+        <v>199</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1136,7 +1115,7 @@
         <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1144,10 +1123,10 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1155,10 +1134,10 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>54</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1166,10 +1145,10 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1177,10 +1156,10 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1188,10 +1167,10 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1199,10 +1178,10 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>249</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1210,10 +1189,10 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1221,208 +1200,208 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="B40">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B41">
-        <v>29</v>
+        <v>248</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B42">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B43">
         <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B45">
-        <v>149</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B47">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B48">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C48" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B49">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B50">
-        <v>109</v>
+        <v>199</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B51">
-        <v>179</v>
+        <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B52">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="C52" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B53">
-        <v>197</v>
+        <v>16</v>
       </c>
       <c r="C53" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C54" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55">
-        <v>29</v>
+        <v>179</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B57">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1430,10 +1409,10 @@
         <v>54</v>
       </c>
       <c r="B58">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1441,10 +1420,10 @@
         <v>55</v>
       </c>
       <c r="B59">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="C59" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1452,10 +1431,10 @@
         <v>56</v>
       </c>
       <c r="B60">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1463,10 +1442,10 @@
         <v>57</v>
       </c>
       <c r="B61">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1474,10 +1453,10 @@
         <v>58</v>
       </c>
       <c r="B62">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1485,21 +1464,21 @@
         <v>59</v>
       </c>
       <c r="B63">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C63" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B64">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="C64" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1507,10 +1486,10 @@
         <v>60</v>
       </c>
       <c r="B65">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C65" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1518,10 +1497,10 @@
         <v>61</v>
       </c>
       <c r="B66">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C66" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1529,10 +1508,10 @@
         <v>62</v>
       </c>
       <c r="B67">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C67" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1540,10 +1519,10 @@
         <v>63</v>
       </c>
       <c r="B68">
-        <v>199</v>
+        <v>259</v>
       </c>
       <c r="C68" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1551,10 +1530,10 @@
         <v>64</v>
       </c>
       <c r="B69">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1562,10 +1541,10 @@
         <v>65</v>
       </c>
       <c r="B70">
-        <v>269</v>
+        <v>35</v>
       </c>
       <c r="C70" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1573,10 +1552,10 @@
         <v>66</v>
       </c>
       <c r="B71">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C71" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1584,10 +1563,10 @@
         <v>67</v>
       </c>
       <c r="B72">
-        <v>182</v>
+        <v>749</v>
       </c>
       <c r="C72" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1595,10 +1574,10 @@
         <v>68</v>
       </c>
       <c r="B73">
-        <v>99</v>
+        <v>598</v>
       </c>
       <c r="C73" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1606,10 +1585,10 @@
         <v>69</v>
       </c>
       <c r="B74">
-        <v>120</v>
+        <v>279</v>
       </c>
       <c r="C74" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1617,10 +1596,10 @@
         <v>70</v>
       </c>
       <c r="B75">
-        <v>73</v>
+        <v>849</v>
       </c>
       <c r="C75" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1628,10 +1607,10 @@
         <v>71</v>
       </c>
       <c r="B76">
-        <v>76</v>
+        <v>449</v>
       </c>
       <c r="C76" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1639,10 +1618,10 @@
         <v>72</v>
       </c>
       <c r="B77">
-        <v>32</v>
+        <v>348</v>
       </c>
       <c r="C77" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1650,10 +1629,10 @@
         <v>73</v>
       </c>
       <c r="B78">
-        <v>51</v>
+        <v>449</v>
       </c>
       <c r="C78" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1661,10 +1640,10 @@
         <v>74</v>
       </c>
       <c r="B79">
-        <v>86</v>
+        <v>234</v>
       </c>
       <c r="C79" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1672,10 +1651,10 @@
         <v>75</v>
       </c>
       <c r="B80">
-        <v>49</v>
+        <v>798</v>
       </c>
       <c r="C80" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1683,10 +1662,10 @@
         <v>76</v>
       </c>
       <c r="B81">
-        <v>84</v>
+        <v>399</v>
       </c>
       <c r="C81" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1694,10 +1673,10 @@
         <v>77</v>
       </c>
       <c r="B82">
-        <v>199</v>
+        <v>899</v>
       </c>
       <c r="C82" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1705,10 +1684,10 @@
         <v>78</v>
       </c>
       <c r="B83">
-        <v>349</v>
+        <v>248</v>
       </c>
       <c r="C83" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1716,10 +1695,10 @@
         <v>79</v>
       </c>
       <c r="B84">
-        <v>116</v>
+        <v>379</v>
       </c>
       <c r="C84" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1727,516 +1706,417 @@
         <v>80</v>
       </c>
       <c r="B85">
-        <v>69</v>
+        <v>149</v>
       </c>
       <c r="C85" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B86">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="C86" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B87">
-        <v>32</v>
+        <v>449</v>
       </c>
       <c r="C87" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B88">
-        <v>128</v>
+        <v>269</v>
       </c>
       <c r="C88" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B89">
-        <v>70</v>
+        <v>1999</v>
       </c>
       <c r="C89" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B90">
-        <v>79</v>
+        <v>349</v>
       </c>
       <c r="C90" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B91">
-        <v>197</v>
+        <v>498</v>
       </c>
       <c r="C91" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B92">
-        <v>112</v>
+        <v>797</v>
       </c>
       <c r="C92" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B93">
-        <v>338</v>
+        <v>269</v>
       </c>
       <c r="C93" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B94">
-        <v>17</v>
+        <v>798</v>
       </c>
       <c r="C94" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B95">
-        <v>139</v>
+        <v>749</v>
       </c>
       <c r="C95" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B96">
-        <v>23</v>
+        <v>579</v>
       </c>
       <c r="C96" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B97">
-        <v>25</v>
+        <v>238</v>
       </c>
       <c r="C97" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B98">
-        <v>66</v>
+        <v>428</v>
       </c>
       <c r="C98" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B99">
-        <v>261</v>
+        <v>698</v>
       </c>
       <c r="C99" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B100">
-        <v>149</v>
+        <v>328</v>
       </c>
       <c r="C100" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B101">
-        <v>171</v>
+        <v>1998</v>
       </c>
       <c r="C101" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B102">
-        <v>159</v>
+        <v>1399</v>
       </c>
       <c r="C102" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B103">
-        <v>44</v>
+        <v>2197</v>
       </c>
       <c r="C103" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B104">
-        <v>999</v>
+        <v>1498</v>
       </c>
       <c r="C104" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B105">
-        <v>408</v>
+        <v>1398</v>
       </c>
       <c r="C105" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B106">
-        <v>253</v>
+        <v>1798</v>
       </c>
       <c r="C106" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="B107">
-        <v>49</v>
+        <v>847</v>
       </c>
       <c r="C107" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B108">
-        <v>89</v>
+        <v>428</v>
       </c>
       <c r="C108" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B109">
-        <v>24</v>
+        <v>1449</v>
       </c>
       <c r="C109" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B110">
-        <v>129</v>
+        <v>329</v>
       </c>
       <c r="C110" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B111">
-        <v>260</v>
+        <v>2997</v>
       </c>
       <c r="C111" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B112">
-        <v>119</v>
+        <v>1598</v>
       </c>
       <c r="C112" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B113">
-        <v>54</v>
+        <v>4998</v>
       </c>
       <c r="C113" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B114">
-        <v>49</v>
+        <v>749</v>
       </c>
       <c r="C114" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B115">
-        <v>279</v>
+        <v>499</v>
       </c>
       <c r="C115" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B116">
-        <v>299</v>
+        <v>696</v>
       </c>
       <c r="C116" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B117">
-        <v>155</v>
+        <v>899</v>
       </c>
       <c r="C117" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B118">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="C118" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B119">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="C119" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B120">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="C120" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B121">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="C121" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B122">
-        <v>150</v>
+        <v>21</v>
       </c>
       <c r="C122" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" t="s">
-        <v>115</v>
-      </c>
-      <c r="B123">
-        <v>45</v>
-      </c>
-      <c r="C123" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" t="s">
-        <v>116</v>
-      </c>
-      <c r="B124">
-        <v>279</v>
-      </c>
-      <c r="C124" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" t="s">
-        <v>117</v>
-      </c>
-      <c r="B125">
-        <v>17</v>
-      </c>
-      <c r="C125" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" t="s">
-        <v>118</v>
-      </c>
-      <c r="B126">
-        <v>197</v>
-      </c>
-      <c r="C126" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" t="s">
-        <v>119</v>
-      </c>
-      <c r="B127">
-        <v>54</v>
-      </c>
-      <c r="C127" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" t="s">
-        <v>120</v>
-      </c>
-      <c r="B128">
-        <v>9</v>
-      </c>
-      <c r="C128" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129" t="s">
-        <v>121</v>
-      </c>
-      <c r="B129">
-        <v>56</v>
-      </c>
-      <c r="C129" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130" t="s">
-        <v>122</v>
-      </c>
-      <c r="B130">
-        <v>22</v>
-      </c>
-      <c r="C130" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131" t="s">
-        <v>123</v>
-      </c>
-      <c r="B131">
-        <v>67</v>
-      </c>
-      <c r="C131" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>